<commit_message>
Se genera el presupuesto con kicost
</commit_message>
<xml_diff>
--- a/PonchoEDUCIAA_WIFI_BLT.xlsx
+++ b/PonchoEDUCIAA_WIFI_BLT.xlsx
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="184">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -612,19 +612,19 @@
     <t>R1,R4,R5</t>
   </si>
   <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>RES SMD 400 OHM 0.1% 0.15W 0603</t>
-  </si>
-  <si>
-    <t>Resistors_SMD:R_1206_HandSoldering</t>
-  </si>
-  <si>
-    <t>Vishay Thin Film</t>
-  </si>
-  <si>
-    <t>PAT0603E4000BST1</t>
+    <t>402</t>
+  </si>
+  <si>
+    <t>RES SMD 402 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>Resistors_SMD:R_0805_HandSoldering</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0805FR-07402RL</t>
   </si>
   <si>
     <t>D2</t>
@@ -738,13 +738,10 @@
     <t>470</t>
   </si>
   <si>
-    <t>RES SMD 470 OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics Inc.</t>
-  </si>
-  <si>
-    <t>RMCF0402FT470R</t>
+    <t>RES SMD 470 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-07470RL</t>
   </si>
   <si>
     <t>R2</t>
@@ -753,13 +750,13 @@
     <t>10k</t>
   </si>
   <si>
-    <t>10k Ohm Â±0.1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thin Film</t>
-  </si>
-  <si>
-    <t>TE Connectivity Passive Product</t>
-  </si>
-  <si>
-    <t>CPF0402B10KE1</t>
+    <t>RES SMD 10K OHM 0.1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ERA-6AEB103V</t>
   </si>
   <si>
     <t>C4</t>
@@ -783,19 +780,19 @@
     <t>0201ZA101JAT2A</t>
   </si>
   <si>
-    <t>R7</t>
+    <t>R7,R8</t>
   </si>
   <si>
     <t>5k</t>
   </si>
   <si>
-    <t>RES SMD 5K OHM 0.05% 1/4W 1206</t>
+    <t>RES SMD 5K OHM 1% 1/8W 0805</t>
   </si>
   <si>
     <t>Vishay Dale</t>
   </si>
   <si>
-    <t>TNPU12065K00AZEN00</t>
+    <t>CRCW08055K00FKTA</t>
   </si>
   <si>
     <t>SW1</t>
@@ -873,7 +870,7 @@
     <t>952-1386-ND</t>
   </si>
   <si>
-    <t>PAT400ACT-ND</t>
+    <t>311-402CRCT-ND</t>
   </si>
   <si>
     <t>350-2814-ND</t>
@@ -897,10 +894,10 @@
     <t>478-5266-1-ND</t>
   </si>
   <si>
-    <t>RMCF0402FT470RCT-ND</t>
-  </si>
-  <si>
-    <t>A102579CT-ND</t>
+    <t>311-470CRCT-ND</t>
+  </si>
+  <si>
+    <t>P10KDACT-ND</t>
   </si>
   <si>
     <t>490-5921-1-ND</t>
@@ -909,7 +906,7 @@
     <t>478-1026-1-ND</t>
   </si>
   <si>
-    <t>541-3307-1-ND</t>
+    <t>CRCW08055K00FKTA-ND</t>
   </si>
   <si>
     <t>401-1969-ND</t>
@@ -939,12 +936,18 @@
     <t>1657913</t>
   </si>
   <si>
-    <t>1697334</t>
+    <t>9237445</t>
+  </si>
+  <si>
+    <t>1577673</t>
   </si>
   <si>
     <t>2218834</t>
   </si>
   <si>
+    <t>2616759</t>
+  </si>
+  <si>
     <t>1201381</t>
   </si>
   <si>
@@ -954,24 +957,27 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>534-3320</t>
+    <t>485-3320</t>
   </si>
   <si>
     <t>855-M50-3501042</t>
   </si>
   <si>
-    <t>71-PAT0603E4000BST1</t>
+    <t>603-RC0805FR-07402RL</t>
   </si>
   <si>
     <t>645-561-2201-050F</t>
   </si>
   <si>
-    <t>Not Assigned</t>
+    <t>645-550-0804F</t>
   </si>
   <si>
     <t>645-550-0504F</t>
   </si>
   <si>
+    <t>538-22-27-2031</t>
+  </si>
+  <si>
     <t>81-GRM1555C1H101JA1D</t>
   </si>
   <si>
@@ -981,7 +987,10 @@
     <t>581-02016D104KAT2A</t>
   </si>
   <si>
-    <t>279-CPF0402B10KE1</t>
+    <t>603-RC0805FR-07470RL</t>
+  </si>
+  <si>
+    <t>667-ERA-6AEB103V</t>
   </si>
   <si>
     <t>81-GRM1555C1H100JA1D</t>
@@ -990,6 +999,9 @@
     <t>581-0201ZA101JAT2A</t>
   </si>
   <si>
+    <t>71-CRCW08055K60JNEB</t>
+  </si>
+  <si>
     <t>611-D6C90F1LFS</t>
   </si>
   <si>
@@ -1005,7 +1017,7 @@
     <t>74K2300</t>
   </si>
   <si>
-    <t>06Y8762</t>
+    <t>66R3296</t>
   </si>
   <si>
     <t>30K3275</t>
@@ -1017,7 +1029,7 @@
     <t>13T6895</t>
   </si>
   <si>
-    <t>48W5738</t>
+    <t>03AC2607</t>
   </si>
   <si>
     <t>03AC2742</t>
@@ -1026,7 +1038,10 @@
     <t>85K9474</t>
   </si>
   <si>
-    <t>80P3854</t>
+    <t>89K7298</t>
+  </si>
+  <si>
+    <t>08N2142</t>
   </si>
   <si>
     <t>48W5737</t>
@@ -1035,6 +1050,9 @@
     <t>55J0850</t>
   </si>
   <si>
+    <t>49H8224</t>
+  </si>
+  <si>
     <t>99R3435</t>
   </si>
   <si>
@@ -1065,7 +1083,10 @@
     <t>698-2995</t>
   </si>
   <si>
-    <t>701-5024</t>
+    <t>618-2546</t>
+  </si>
+  <si>
+    <t>565-948</t>
   </si>
   <si>
     <t>776-9194</t>
@@ -1590,7 +1611,7 @@
   <sheetData>
     <row r="1" spans="1:39">
       <c r="H1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I1" s="2">
         <v>100</v>
@@ -1598,7 +1619,7 @@
     </row>
     <row r="2" spans="1:39">
       <c r="H2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" s="4">
         <f>sum(I7:I24)</f>
@@ -1627,7 +1648,7 @@
     </row>
     <row r="3" spans="1:39">
       <c r="H3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" s="5">
         <f>TotalCost/BoardQty</f>
@@ -1647,7 +1668,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -1655,7 +1676,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -1663,7 +1684,7 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
@@ -1671,7 +1692,7 @@
       <c r="Z5" s="9"/>
       <c r="AA5" s="9"/>
       <c r="AB5" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="AC5" s="10"/>
       <c r="AD5" s="10"/>
@@ -1679,7 +1700,7 @@
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
       <c r="AH5" s="11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="AI5" s="11"/>
       <c r="AJ5" s="11"/>
@@ -1716,10 +1737,10 @@
         <v>9</v>
       </c>
       <c r="J6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>8</v>
@@ -1728,16 +1749,16 @@
         <v>9</v>
       </c>
       <c r="N6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="O6" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="P6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>8</v>
@@ -1746,16 +1767,16 @@
         <v>9</v>
       </c>
       <c r="T6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="U6" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="U6" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="V6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="W6" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="W6" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="X6" s="12" t="s">
         <v>8</v>
@@ -1764,16 +1785,16 @@
         <v>9</v>
       </c>
       <c r="Z6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA6" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AA6" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="AB6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC6" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="AC6" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="AD6" s="12" t="s">
         <v>8</v>
@@ -1782,16 +1803,16 @@
         <v>9</v>
       </c>
       <c r="AF6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG6" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AG6" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="AH6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI6" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="AI6" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="AJ6" s="12" t="s">
         <v>8</v>
@@ -1800,10 +1821,10 @@
         <v>9</v>
       </c>
       <c r="AL6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM6" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="AM6" s="12" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:39">
@@ -1841,7 +1862,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="13">
-        <f>iferror(lookup(if(K7="",G7,K7),{0,1},{0.0,6.71}),"")</f>
+        <f>iferror(lookup(if(K7="",G7,K7),{0,1},{0.0,8.95}),"")</f>
         <v>0</v>
       </c>
       <c r="M7" s="13">
@@ -1849,10 +1870,10 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R7" s="13">
         <f>iferror(lookup(if(Q7="",G7,Q7),{0,1,5,15,25,75,150,250,500},{0.0,1.7752099999999997,1.62639,1.4775699999999998,1.43505,1.39253,1.35001,1.33938,1.31812}),"")</f>
@@ -1863,16 +1884,16 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V7">
-        <v>790</v>
+        <v>7</v>
       </c>
       <c r="X7" s="13">
-        <f>iferror(lookup(if(W7="",G7,W7),{0,1,10,50,100,200,500,1000,2500,5000},{0.0,0.172,0.167,0.126,0.117,0.103,0.099,0.081,0.073,0.071}),"")</f>
+        <f>iferror(lookup(if(W7="",G7,W7),{0,1,10},{0.0,8.97,8.08}),"")</f>
         <v>0</v>
       </c>
       <c r="Y7" s="13">
@@ -1880,25 +1901,25 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AF7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="AG7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH7">
         <v>60</v>
       </c>
       <c r="AL7" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="AM7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:39">
@@ -1933,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>2781</v>
+        <v>2552</v>
       </c>
       <c r="L8" s="13">
         <f>iferror(lookup(if(K8="",G8,K8),{0,1,10,100,500,1000,5000,10000},{0.0,2.0,1.815,1.5561,1.29676,1.1115,0.98553,0.9633}),"")</f>
@@ -1944,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R8" s="13">
         <f>iferror(lookup(if(Q8="",G8,Q8),{0,1,5,50,100,250,500,1000,2500},{0.0,1.63702,1.63702,1.5945,1.55198,1.40316,1.29686,1.11615,0.98859}),"")</f>
@@ -1958,16 +1979,16 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V8">
-        <v>3638</v>
+        <v>3558</v>
       </c>
       <c r="X8" s="13">
-        <f>iferror(lookup(if(W8="",G8,W8),{0,1,10,100,250,500,1000},{0.0,2.0,1.63,1.55,1.4,1.29,1.14}),"")</f>
+        <f>iferror(lookup(if(W8="",G8,W8),{0,1,10,100,250,500,1000},{0.0,2.0,1.64,1.56,1.4,1.29,1.21}),"")</f>
         <v>0</v>
       </c>
       <c r="Y8" s="13">
@@ -1975,10 +1996,10 @@
         <v>0</v>
       </c>
       <c r="Z8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AA8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD8" s="13">
         <f>iferror(lookup(if(AC8="",G8,AC8),{0,1,10,50,100,250,500,1000,2500},{0.0,2.0,1.82,1.67,1.56,1.49,1.34,1.23,1.12}),"")</f>
@@ -1989,13 +2010,13 @@
         <v>0</v>
       </c>
       <c r="AF8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="AG8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH8">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="AJ8" s="13">
         <f>iferror(lookup(if(AI8="",G8,AI8),{0,1,10},{0.0,1.71143,1.67954}),"")</f>
@@ -2006,10 +2027,10 @@
         <v>0</v>
       </c>
       <c r="AL8" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="AM8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:39">
@@ -2044,10 +2065,10 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>7927</v>
+        <v>101602</v>
       </c>
       <c r="L9" s="13">
-        <f>iferror(lookup(if(K9="",G9,K9),{0,1,10,100,1000},{0.0,0.97,0.839,0.5844,0.319}),"")</f>
+        <f>iferror(lookup(if(K9="",G9,K9),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0.0,0.1,0.022,0.0088,0.00396,0.00344,0.00284,0.00247,0.00217,0.00199,0.00195}),"")</f>
         <v>0</v>
       </c>
       <c r="M9" s="13">
@@ -2055,13 +2076,16 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="V9">
+        <v>47564</v>
       </c>
       <c r="X9" s="13">
-        <f>iferror(lookup(if(W9="",G9,W9),{0,1,25,100,250,500,1000,5000},{0.0,0.79,0.64,0.555,0.483,0.401,0.289,0.285}),"")</f>
+        <f>iferror(lookup(if(W9="",G9,W9),{0,1,10,100,1000,5000,25000},{0.0,0.101,0.016,0.006,0.004,0.003,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y9" s="13">
@@ -2069,13 +2093,13 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AA9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD9" s="13">
-        <f>iferror(lookup(if(AC9="",G9,AC9),{0,1,1000,2000,3000},{0.0,0.443,0.443,0.415,0.392}),"")</f>
+        <f>iferror(lookup(if(AC9="",G9,AC9),{0,1,5000,10000,15000},{0.0,0.005,0.005,0.004,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AE9" s="13">
@@ -2083,10 +2107,10 @@
         <v>0</v>
       </c>
       <c r="AF9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="AG9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:39">
@@ -2132,16 +2156,16 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V10">
-        <v>1020</v>
+        <v>1010</v>
       </c>
       <c r="X10" s="13">
-        <f>iferror(lookup(if(W10="",G10,W10),{0,1,10,100,500,1000,2500,5000,10000},{0.0,1.23,0.773,0.618,0.525,0.432,0.411,0.402,0.401}),"")</f>
+        <f>iferror(lookup(if(W10="",G10,W10),{0,1,10,100,500,1000,2500,5000},{0.0,1.23,0.775,0.619,0.526,0.435,0.412,0.403}),"")</f>
         <v>0</v>
       </c>
       <c r="Y10" s="13">
@@ -2149,10 +2173,10 @@
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AA10" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD10" s="13">
         <f>iferror(lookup(if(AC10="",G10,AC10),{0,1,1625},{0.0,0.433,0.433}),"")</f>
@@ -2163,10 +2187,10 @@
         <v>0</v>
       </c>
       <c r="AF10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="AG10" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:39">
@@ -2212,16 +2236,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="V11">
+        <v>340</v>
+      </c>
+      <c r="X11" s="13">
+        <f>iferror(lookup(if(W11="",G11,W11),{0,1,10,100,500,1000,2500,5000},{0.0,1.76,1.09,0.876,0.745,0.614,0.582,0.569}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="13">
+        <f>iferror(if(W11="",G11,W11)*X11,"")</f>
+        <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AA11" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD11" s="13">
         <f>iferror(lookup(if(AC11="",G11,AC11),{0,1,10,25,50,100,250,500,1000},{0.0,1.75,1.09,1.02,0.946,0.874,0.809,0.743,0.612}),"")</f>
@@ -2232,13 +2267,13 @@
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="AG11" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH11">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="AJ11" s="13">
         <f>iferror(lookup(if(AI11="",G11,AI11),{0,1,25,100,250,500},{0.0,1.3606399999999998,0.8504,0.69095,0.6271699999999999,0.57402}),"")</f>
@@ -2249,10 +2284,10 @@
         <v>0</v>
       </c>
       <c r="AL11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="AM11" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:39">
@@ -2287,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>997</v>
+        <v>992</v>
       </c>
       <c r="L12" s="13">
-        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500,1000,2500,5000},{0.0,1.75,1.42,1.0924,0.9833,0.874,0.7429,0.6118,0.58121,0.5681}),"")</f>
+        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500},{0.0,1.75,1.42,1.0924,0.9833,0.874,0.7429}),"")</f>
         <v>0</v>
       </c>
       <c r="M12" s="13">
@@ -2298,16 +2333,16 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V12">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="X12" s="13">
-        <f>iferror(lookup(if(W12="",G12,W12),{0,1,10,100,500,1000,2500,5000},{0.0,1.75,1.09,0.873,0.743,0.612,0.581,0.568}),"")</f>
+        <f>iferror(lookup(if(W12="",G12,W12),{0,1,10,100,500,1000,2500,5000},{0.0,1.76,1.09,0.876,0.745,0.614,0.582,0.569}),"")</f>
         <v>0</v>
       </c>
       <c r="Y12" s="13">
@@ -2315,10 +2350,10 @@
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AA12" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH12">
         <v>22</v>
@@ -2332,10 +2367,10 @@
         <v>0</v>
       </c>
       <c r="AL12" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AM12" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:39">
@@ -2370,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>18056</v>
+        <v>48007</v>
       </c>
       <c r="L13" s="13">
         <f>iferror(lookup(if(K13="",G13,K13),{0,1,10,25,50,100,250,500,1000,2500},{0.0,0.35,0.334,0.2864,0.2436,0.234,0.21012,0.20056,0.16713,0.1528}),"")</f>
@@ -2381,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R13" s="13">
         <f>iferror(lookup(if(Q13="",G13,Q13),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.243427,0.243427,0.210474,0.167954,0.15307199999999999,0.143505,0.13819,0.133938}),"")</f>
@@ -2395,19 +2430,30 @@
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="V13">
+        <v>25266</v>
+      </c>
+      <c r="X13" s="13">
+        <f>iferror(lookup(if(W13="",G13,W13),{0,1,10,100,500,1000,2500,10000,25000,50000},{0.0,0.361,0.269,0.233,0.202,0.168,0.153,0.134,0.129,0.125}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="13">
+        <f>iferror(if(W13="",G13,W13)*X13,"")</f>
+        <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AA13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD13" s="13">
-        <f>iferror(lookup(if(AC13="",G13,AC13),{0,1,10,100,500,1000,2500,5000,10000},{0.0,0.33,0.243,0.21,0.167,0.153,0.143,0.138,0.134}),"")</f>
+        <f>iferror(lookup(if(AC13="",G13,AC13),{0,1,10,100,500,1000,5000,10000},{0.0,0.33,0.243,0.21,0.167,0.153,0.138,0.134}),"")</f>
         <v>0</v>
       </c>
       <c r="AE13" s="13">
@@ -2415,10 +2461,10 @@
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="AG13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:39">
@@ -2453,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>2412242</v>
+        <v>1848285</v>
       </c>
       <c r="L14" s="13">
         <f>iferror(lookup(if(K14="",G14,K14),{0,1,10,100,500,1000,2500,5000,10000,20000,30000},{0.0,0.1,0.014,0.0062,0.00442,0.00348,0.00316,0.00291,0.00231,0.0022,0.00209}),"")</f>
@@ -2464,10 +2510,10 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R14" s="13">
         <f>iferror(lookup(if(Q14="",G14,Q14),{0,1,100,500,2500,5000},{0.0,0.006909499999999999,0.006909499999999999,0.0054213,0.0041456999999999996,0.0038267999999999996}),"")</f>
@@ -2478,16 +2524,16 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V14">
-        <v>1204813</v>
+        <v>689964</v>
       </c>
       <c r="X14" s="13">
-        <f>iferror(lookup(if(W14="",G14,W14),{0,1,10,100,500,2500,10000},{0.0,0.1,0.006,0.004,0.003,0.002,0.002}),"")</f>
+        <f>iferror(lookup(if(W14="",G14,W14),{0,1,10,100,500,2500,10000},{0.0,0.101,0.006,0.004,0.003,0.002,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y14" s="13">
@@ -2495,13 +2541,13 @@
         <v>0</v>
       </c>
       <c r="Z14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AA14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD14" s="13">
-        <f>iferror(lookup(if(AC14="",G14,AC14),{0,1,10,25,50,100,250,500},{0.0,0.006,0.006,0.005,0.005,0.004,0.004,0.003}),"")</f>
+        <f>iferror(lookup(if(AC14="",G14,AC14),{0,1,10000,20000},{0.0,0.003,0.003,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AE14" s="13">
@@ -2509,13 +2555,13 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="AG14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH14">
-        <v>2200</v>
+        <v>1600</v>
       </c>
       <c r="AJ14" s="13">
         <f>iferror(lookup(if(AI14="",G14,AI14),{0,1,200,1000},{0.0,0.006378,0.006378,0.004252}),"")</f>
@@ -2526,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="AL14" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="AM14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:39">
@@ -2564,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>706246</v>
+        <v>616770</v>
       </c>
       <c r="L15" s="13">
         <f>iferror(lookup(if(K15="",G15,K15),{0,1,10,100,500,1000,4000,8000,12000},{0.0,0.15,0.105,0.0495,0.03472,0.02875,0.02129,0.0198,0.01881}),"")</f>
@@ -2575,10 +2621,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R15" s="13">
         <f>iferror(lookup(if(Q15="",G15,Q15),{0,1,100,500,1000,2000},{0.0,0.081851,0.081851,0.066969,0.06144139999999999,0.0566579}),"")</f>
@@ -2589,16 +2635,16 @@
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V15">
-        <v>58327</v>
+        <v>52280</v>
       </c>
       <c r="X15" s="13">
-        <f>iferror(lookup(if(W15="",G15,W15),{0,1,10,100,500,1000,4000},{0.0,0.24,0.113,0.064,0.057,0.048,0.036}),"")</f>
+        <f>iferror(lookup(if(W15="",G15,W15),{0,1,10,100,500,1000,4000},{0.0,0.241,0.113,0.064,0.057,0.048,0.036}),"")</f>
         <v>0</v>
       </c>
       <c r="Y15" s="13">
@@ -2606,13 +2652,13 @@
         <v>0</v>
       </c>
       <c r="Z15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AA15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD15" s="13">
-        <f>iferror(lookup(if(AC15="",G15,AC15),{0,1,4000,5000},{0.0,0.088,0.088,0.08}),"")</f>
+        <f>iferror(lookup(if(AC15="",G15,AC15),{0,1,4000,8000,16000,24000,40000},{0.0,0.051,0.051,0.047,0.044,0.042,0.042}),"")</f>
         <v>0</v>
       </c>
       <c r="AE15" s="13">
@@ -2620,16 +2666,16 @@
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="AG15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH15">
         <v>275</v>
       </c>
       <c r="AJ15" s="13">
-        <f>iferror(lookup(if(AI15="",G15,AI15),{0,1,25,125},{0.0,0.125434,0.125434,0.083977}),"")</f>
+        <f>iferror(lookup(if(AI15="",G15,AI15),{0,1,25,125},{0.0,0.133938,0.133938,0.090355}),"")</f>
         <v>0</v>
       </c>
       <c r="AK15" s="13">
@@ -2637,10 +2683,10 @@
         <v>0</v>
       </c>
       <c r="AL15" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="AM15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:39">
@@ -2675,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>572708</v>
+        <v>117</v>
       </c>
       <c r="L16" s="13">
         <f>iferror(lookup(if(K16="",G16,K16),{0,1,10,100,500,1000,2500,5000,15000,30000},{0.0,0.1,0.011,0.005,0.00354,0.00278,0.00253,0.00233,0.00176,0.00167}),"")</f>
@@ -2686,10 +2732,10 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R16" s="13">
         <f>iferror(lookup(if(Q16="",G16,Q16),{0,1,100,500,2500,7500},{0.0,0.023704899999999998,0.023704899999999998,0.014775699999999998,0.009885899999999998,0.008504}),"")</f>
@@ -2700,16 +2746,16 @@
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V16">
-        <v>164492</v>
+        <v>6348</v>
       </c>
       <c r="X16" s="13">
-        <f>iferror(lookup(if(W16="",G16,W16),{0,1,100,1000,15000},{0.0,0.1,0.039,0.023,0.002}),"")</f>
+        <f>iferror(lookup(if(W16="",G16,W16),{0,1,100,1000,15000},{0.0,0.101,0.039,0.024,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y16" s="13">
@@ -2717,10 +2763,10 @@
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AA16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD16" s="13">
         <f>iferror(lookup(if(AC16="",G16,AC16),{0,1,25,100,250,500,1000},{0.0,0.1,0.07,0.039,0.034,0.028,0.023}),"")</f>
@@ -2731,13 +2777,13 @@
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="AG16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH16">
-        <v>13200</v>
+        <v>13100</v>
       </c>
       <c r="AJ16" s="13">
         <f>iferror(lookup(if(AI16="",G16,AI16),{0,1,100,1000},{0.0,0.052087,0.052087,0.030827}),"")</f>
@@ -2748,10 +2794,10 @@
         <v>0</v>
       </c>
       <c r="AL16" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="AM16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:39">
@@ -2768,10 +2814,10 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
         <v>66</v>
-      </c>
-      <c r="F17" t="s">
-        <v>67</v>
       </c>
       <c r="G17">
         <f>BoardQty*2</f>
@@ -2786,10 +2832,10 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>42771</v>
+        <v>1202983</v>
       </c>
       <c r="L17" s="13">
-        <f>iferror(lookup(if(K17="",G17,K17),{0,1,10,100,1000,2500,5000,10000,30000,50000,100000},{0.0,0.1,0.02,0.0081,0.00364,0.00316,0.00261,0.00227,0.00199,0.00183,0.00181}),"")</f>
+        <f>iferror(lookup(if(K17="",G17,K17),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0.0,0.1,0.022,0.0088,0.00396,0.00344,0.00284,0.00247,0.00217,0.00199,0.00195}),"")</f>
         <v>0</v>
       </c>
       <c r="M17" s="13">
@@ -2797,30 +2843,92 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="R17" s="13">
+        <f>iferror(lookup(if(Q17="",G17,Q17),{0,1,100,500,1000,2500},{0.0,0.0126497,0.0126497,0.009460699999999999,0.0075473,0.0062717}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="13">
+        <f>iferror(if(Q17="",G17,Q17)*R17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="V17">
+        <v>66451</v>
+      </c>
+      <c r="X17" s="13">
+        <f>iferror(lookup(if(W17="",G17,W17),{0,1,10,100,1000,5000,25000},{0.0,0.101,0.016,0.006,0.004,0.003,0.002}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="13">
+        <f>iferror(if(W17="",G17,W17)*X17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD17" s="13">
+        <f>iferror(lookup(if(AC17="",G17,AC17),{0,1,10,25,100,250,1000},{0.0,0.026,0.026,0.018,0.011,0.008,0.006}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="13">
+        <f>iferror(if(AC17="",G17,AC17)*AD17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH17">
+        <v>4</v>
+      </c>
+      <c r="AJ17" s="13">
+        <f>iferror(lookup(if(AI17="",G17,AI17),{0,1,5},{0.0,23.364739999999998,19.293449999999996}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK17" s="13">
+        <f>iferror(if(AI17="",G17,AI17)*AJ17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>180</v>
+      </c>
+      <c r="AM17" s="14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:39">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
       <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
         <v>71</v>
-      </c>
-      <c r="F18" t="s">
-        <v>72</v>
       </c>
       <c r="G18">
         <f>BoardQty*1</f>
@@ -2835,10 +2943,10 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>92751</v>
+        <v>540440</v>
       </c>
       <c r="L18" s="13">
-        <f>iferror(lookup(if(K18="",G18,K18),{0,1,10,100,1000,2000,2500,5000},{0.0,0.58,0.415,0.2158,0.10562,0.10419,0.10824,0.0984}),"")</f>
+        <f>iferror(lookup(if(K18="",G18,K18),{0,1,10,100,1000,2500,5000,10000,25000},{0.0,0.36,0.302,0.1182,0.04948,0.04536,0.03749,0.03499,0.03451}),"")</f>
         <v>0</v>
       </c>
       <c r="M18" s="13">
@@ -2846,13 +2954,13 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R18" s="13">
-        <f>iferror(lookup(if(Q18="",G18,Q18),{0,1,100,250,500},{0.0,0.22960799999999998,0.22960799999999998,0.196655,0.18708799999999998}),"")</f>
+        <f>iferror(lookup(if(Q18="",G18,Q18),{0,1,100,500,1000,2500},{0.0,0.126497,0.126497,0.107363,0.0656934,0.0575083}),"")</f>
         <v>0</v>
       </c>
       <c r="S18" s="13">
@@ -2863,13 +2971,13 @@
         <v>132</v>
       </c>
       <c r="U18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V18">
-        <v>14949</v>
+        <v>67154</v>
       </c>
       <c r="X18" s="13">
-        <f>iferror(lookup(if(W18="",G18,W18),{0,1,10,25,50,100,250,500,1000,2000},{0.0,0.293,0.275,0.248,0.219,0.211,0.192,0.183,0.152,0.137}),"")</f>
+        <f>iferror(lookup(if(W18="",G18,W18),{0,1,10,100,500,1000,5000,10000,25000},{0.0,0.632,0.25,0.149,0.105,0.076,0.043,0.039,0.038}),"")</f>
         <v>0</v>
       </c>
       <c r="Y18" s="13">
@@ -2877,13 +2985,13 @@
         <v>0</v>
       </c>
       <c r="Z18" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD18" s="13">
-        <f>iferror(lookup(if(AC18="",G18,AC18),{0,1,10,25,50,100,250,500},{0.0,0.29,0.27,0.25,0.22,0.21,0.19,0.18}),"")</f>
+        <f>iferror(lookup(if(AC18="",G18,AC18),{0,1,25,50,100,250,500,1000},{0.0,0.63,0.249,0.199,0.149,0.127,0.105,0.076}),"")</f>
         <v>0</v>
       </c>
       <c r="AE18" s="13">
@@ -2891,16 +2999,16 @@
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="AG18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH18">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="AJ18" s="13">
-        <f>iferror(lookup(if(AI18="",G18,AI18),{0,1,10,250},{0.0,0.373113,0.373113,0.30720699999999995}),"")</f>
+        <f>iferror(lookup(if(AI18="",G18,AI18),{0,1,5,50},{0.0,0.238112,0.238112,0.136064}),"")</f>
         <v>0</v>
       </c>
       <c r="AK18" s="13">
@@ -2908,21 +3016,21 @@
         <v>0</v>
       </c>
       <c r="AL18" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="AM18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:39">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -2931,7 +3039,7 @@
         <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G19">
         <f>BoardQty*1</f>
@@ -2946,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1463911</v>
+        <v>1076391</v>
       </c>
       <c r="L19" s="13">
         <f>iferror(lookup(if(K19="",G19,K19),{0,1,10,100,500,1000,2500,5000,10000,20000,30000},{0.0,0.1,0.014,0.0062,0.00442,0.00348,0.00316,0.00291,0.00231,0.0022,0.00209}),"")</f>
@@ -2957,10 +3065,10 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R19" s="13">
         <f>iferror(lookup(if(Q19="",G19,Q19),{0,1,100,500,2500,5000},{0.0,0.0070158,0.0070158,0.0055276,0.004252,0.0038267999999999996}),"")</f>
@@ -2974,13 +3082,13 @@
         <v>133</v>
       </c>
       <c r="U19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V19">
-        <v>395084</v>
+        <v>270939</v>
       </c>
       <c r="X19" s="13">
-        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,100,500,2500,10000},{0.0,0.1,0.006,0.004,0.003,0.002,0.002}),"")</f>
+        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,100,500,2500,10000},{0.0,0.101,0.006,0.004,0.003,0.002,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y19" s="13">
@@ -2988,10 +3096,10 @@
         <v>0</v>
       </c>
       <c r="Z19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AA19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD19" s="13">
         <f>iferror(lookup(if(AC19="",G19,AC19),{0,1,10,25,50,100,250,500},{0.0,0.006,0.006,0.005,0.005,0.004,0.004,0.003}),"")</f>
@@ -3002,13 +3110,13 @@
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="AG19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AJ19" s="13">
-        <f>iferror(lookup(if(AI19="",G19,AI19),{0,1,2,5},{0.0,41.053059999999995,39.416039999999995,37.76839}),"")</f>
+        <f>iferror(lookup(if(AI19="",G19,AI19),{0,1,2,5},{0.0,44.66726,36.79043,32.580949999999994}),"")</f>
         <v>0</v>
       </c>
       <c r="AK19" s="13">
@@ -3016,21 +3124,21 @@
         <v>0</v>
       </c>
       <c r="AL19" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="AM19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:39">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -3039,7 +3147,7 @@
         <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20">
         <f>BoardQty*1</f>
@@ -3054,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>30790</v>
+        <v>30580</v>
       </c>
       <c r="L20" s="13">
         <f>iferror(lookup(if(K20="",G20,K20),{0,1,10,100,500,1000,2500,5000,15000,30000},{0.0,0.46,0.316,0.1898,0.14232,0.12018,0.11385,0.10753,0.08525,0.0825}),"")</f>
@@ -3065,16 +3173,16 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V20">
-        <v>26913</v>
+        <v>26463</v>
       </c>
       <c r="X20" s="13">
-        <f>iferror(lookup(if(W20="",G20,W20),{0,1,10,100,500,1000,2500,10000,15000,45000},{0.0,0.4,0.229,0.14,0.126,0.106,0.095,0.086,0.077,0.075}),"")</f>
+        <f>iferror(lookup(if(W20="",G20,W20),{0,1,10,100,500,1000,2500,10000,15000,45000},{0.0,0.401,0.23,0.14,0.127,0.106,0.095,0.086,0.077,0.075}),"")</f>
         <v>0</v>
       </c>
       <c r="Y20" s="13">
@@ -3082,13 +3190,13 @@
         <v>0</v>
       </c>
       <c r="Z20" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AA20" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD20" s="13">
-        <f>iferror(lookup(if(AC20="",G20,AC20),{0,1,15000,30000,75000,105000},{0.0,0.067,0.067,0.065,0.064,0.063}),"")</f>
+        <f>iferror(lookup(if(AC20="",G20,AC20),{0,1,15000,30000,60000},{0.0,0.076,0.076,0.076,0.075}),"")</f>
         <v>0</v>
       </c>
       <c r="AE20" s="13">
@@ -3096,33 +3204,33 @@
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="AG20" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:39">
       <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>82</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
         <v>83</v>
       </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
       <c r="G21">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H21" s="13">
@@ -3133,11 +3241,8 @@
         <f>iferror(G21*H21,"")</f>
         <v>0</v>
       </c>
-      <c r="J21">
-        <v>986</v>
-      </c>
       <c r="L21" s="13">
-        <f>iferror(lookup(if(K21="",G21,K21),{0,1,10,100,1000},{0.0,3.92,3.498,2.5889,1.75682}),"")</f>
+        <f>iferror(lookup(if(K21="",G21,K21),{0,1,50000,125000},{0.0,0.0124,0.0124,0.01212}),"")</f>
         <v>0</v>
       </c>
       <c r="M21" s="13">
@@ -3145,30 +3250,75 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="R21" s="13">
+        <f>iferror(lookup(if(Q21="",G21,Q21),{0,1,10,100,500,1000,2500,5000,25000,50000},{0.0,0.12224499999999999,0.12224499999999999,0.048898,0.041882199999999994,0.024449,0.016263899999999998,0.0122245,0.008185099999999999,0.0070158}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="13">
+        <f>iferror(if(Q21="",G21,Q21)*R21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T21" t="s">
+        <v>134</v>
+      </c>
+      <c r="U21" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="V21">
+        <v>48671</v>
+      </c>
+      <c r="X21" s="13">
+        <f>iferror(lookup(if(W21="",G21,W21),{0,1,10,100,10000,30000},{0.0,0.101,0.047,0.026,0.004,0.003}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="13">
+        <f>iferror(if(W21="",G21,W21)*X21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA21" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD21" s="13">
+        <f>iferror(lookup(if(AC21="",G21,AC21),{0,1,25,50,100,250,500,1000},{0.0,0.17,0.097,0.076,0.055,0.052,0.048,0.045}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="13">
+        <f>iferror(if(AC21="",G21,AC21)*AD21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>169</v>
+      </c>
+      <c r="AG21" s="14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:39">
       <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>88</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>89</v>
-      </c>
-      <c r="F22" t="s">
-        <v>90</v>
       </c>
       <c r="G22">
         <f>BoardQty*1</f>
@@ -3183,10 +3333,10 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>5124</v>
+        <v>6616</v>
       </c>
       <c r="L22" s="13">
-        <f>iferror(lookup(if(K22="",G22,K22),{0,1,10,25,50,100,250,500,1000,5000},{0.0,1.09,1.021,0.972,0.9234,0.8991,0.8748,0.8262,0.7776,0.6561}),"")</f>
+        <f>iferror(lookup(if(K22="",G22,K22),{0,1,10,25,50,100,250,500,1000,5000},{0.0,1.15,1.071,1.02,0.969,0.9435,0.918,0.867,0.816,0.6885}),"")</f>
         <v>0</v>
       </c>
       <c r="M22" s="13">
@@ -3194,10 +3344,10 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R22" s="13">
         <f>iferror(lookup(if(Q22="",G22,Q22),{0,1,20,50,150,400,1250,4000,10000},{0.0,1.09489,1.042803,0.964141,0.930125,0.717525,0.6675639999999999,0.6346109999999999,0.6218549999999999}),"")</f>
@@ -3208,16 +3358,16 @@
         <v>0</v>
       </c>
       <c r="T22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="U22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V22">
-        <v>2579</v>
+        <v>2191</v>
       </c>
       <c r="X22" s="13">
-        <f>iferror(lookup(if(W22="",G22,W22),{0,1,25,50,100,250,500,1000,2000,5000},{0.0,1.08,1.02,0.967,0.941,0.916,0.865,0.814,0.775,0.687}),"")</f>
+        <f>iferror(lookup(if(W22="",G22,W22),{0,1,25,50,100,250,500,1000,2000,5000},{0.0,1.08,1.02,0.969,0.944,0.918,0.867,0.816,0.777,0.689}),"")</f>
         <v>0</v>
       </c>
       <c r="Y22" s="13">
@@ -3225,10 +3375,10 @@
         <v>0</v>
       </c>
       <c r="Z22" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="AA22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD22" s="13">
         <f>iferror(lookup(if(AC22="",G22,AC22),{0,1,10,100,500,1000,5000,10000},{0.0,1.03,0.99,0.951,0.939,0.928,0.917,0.906}),"")</f>
@@ -3239,16 +3389,16 @@
         <v>0</v>
       </c>
       <c r="AF22" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="AG22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AH22">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AJ22" s="13">
-        <f>iferror(lookup(if(AI22="",G22,AI22),{0,1,25,100,250,500},{0.0,1.7008,1.4988299999999999,1.3606399999999998,1.2755999999999998,1.21182}),"")</f>
+        <f>iferror(lookup(if(AI22="",G22,AI22),{0,1,25,100,250,500},{0.0,1.5307199999999999,1.35001,1.2224499999999998,1.14804,1.09489}),"")</f>
         <v>0</v>
       </c>
       <c r="AK22" s="13">
@@ -3256,30 +3406,30 @@
         <v>0</v>
       </c>
       <c r="AL22" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="AM22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:39">
       <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
         <v>91</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>92</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>93</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
         <v>94</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
       </c>
       <c r="G23">
         <f>BoardQty*1</f>
@@ -3294,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>10495</v>
+        <v>5914</v>
       </c>
       <c r="L23" s="13">
         <f>iferror(lookup(if(K23="",G23,K23),{0,1,10,25,50,100,250,500,1000,5000},{0.0,0.41,0.396,0.3876,0.3466,0.33,0.32176,0.27226,0.264,0.231}),"")</f>
@@ -3305,10 +3455,10 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R23" s="13">
         <f>iferror(lookup(if(Q23="",G23,Q23),{0,1,10,40,100,300,900,3000,9000},{0.0,0.41882199999999997,0.396499,0.353979,0.32846699999999995,0.278506,0.27000199999999996,0.264687,0.259372}),"")</f>
@@ -3319,16 +3469,16 @@
         <v>0</v>
       </c>
       <c r="T23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="U23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V23">
-        <v>4626</v>
+        <v>11403</v>
       </c>
       <c r="X23" s="13">
-        <f>iferror(lookup(if(W23="",G23,W23),{0,1,10,50,100,200,500,1000,2000},{0.0,0.4,0.392,0.342,0.326,0.318,0.269,0.261,0.229}),"")</f>
+        <f>iferror(lookup(if(W23="",G23,W23),{0,1,10,50,100,200,500,1000,2000},{0.0,0.401,0.393,0.343,0.328,0.319,0.27,0.262,0.23}),"")</f>
         <v>0</v>
       </c>
       <c r="Y23" s="13">
@@ -3336,13 +3486,13 @@
         <v>0</v>
       </c>
       <c r="Z23" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="AA23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AD23" s="13">
-        <f>iferror(lookup(if(AC23="",G23,AC23),{0,1,250,500,1000,5000},{0.0,0.492,0.371,0.331,0.298,0.271}),"")</f>
+        <f>iferror(lookup(if(AC23="",G23,AC23),{0,1,250,500,1000,5000},{0.0,0.513,0.387,0.345,0.311,0.282}),"")</f>
         <v>0</v>
       </c>
       <c r="AE23" s="13">
@@ -3350,21 +3500,21 @@
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="AG23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:39">
       <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>97</v>
-      </c>
-      <c r="D24" t="s">
-        <v>98</v>
       </c>
       <c r="G24">
         <f>BoardQty*3</f>
@@ -4505,222 +4655,252 @@
     <mergeCell ref="AH5:AM5"/>
   </mergeCells>
   <conditionalFormatting sqref="AD10">
-    <cfRule type="cellIs" dxfId="0" priority="85" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="lessThanOrEqual">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD11">
-    <cfRule type="cellIs" dxfId="0" priority="87" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="99" operator="lessThanOrEqual">
       <formula>H11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD13">
-    <cfRule type="cellIs" dxfId="0" priority="89" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="101" operator="lessThanOrEqual">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD14">
-    <cfRule type="cellIs" dxfId="0" priority="91" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="103" operator="lessThanOrEqual">
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD15">
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="lessThanOrEqual">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD16">
+    <cfRule type="cellIs" dxfId="0" priority="107" operator="lessThanOrEqual">
+      <formula>H16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD17">
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD18">
+    <cfRule type="cellIs" dxfId="0" priority="111" operator="lessThanOrEqual">
+      <formula>H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD19">
+    <cfRule type="cellIs" dxfId="0" priority="113" operator="lessThanOrEqual">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD20">
+    <cfRule type="cellIs" dxfId="0" priority="115" operator="lessThanOrEqual">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD21">
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="lessThanOrEqual">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD22">
+    <cfRule type="cellIs" dxfId="0" priority="119" operator="lessThanOrEqual">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD23">
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="lessThanOrEqual">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD8">
     <cfRule type="cellIs" dxfId="0" priority="93" operator="lessThanOrEqual">
+      <formula>H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD9">
+    <cfRule type="cellIs" dxfId="0" priority="95" operator="lessThanOrEqual">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE10">
+    <cfRule type="cellIs" dxfId="0" priority="98" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE11">
+    <cfRule type="cellIs" dxfId="0" priority="100" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE13">
+    <cfRule type="cellIs" dxfId="0" priority="102" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE14">
+    <cfRule type="cellIs" dxfId="0" priority="104" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE15">
+    <cfRule type="cellIs" dxfId="0" priority="106" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE16">
+    <cfRule type="cellIs" dxfId="0" priority="108" operator="lessThanOrEqual">
+      <formula>I16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE17">
+    <cfRule type="cellIs" dxfId="0" priority="110" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE18">
+    <cfRule type="cellIs" dxfId="0" priority="112" operator="lessThanOrEqual">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE19">
+    <cfRule type="cellIs" dxfId="0" priority="114" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE20">
+    <cfRule type="cellIs" dxfId="0" priority="116" operator="lessThanOrEqual">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE21">
+    <cfRule type="cellIs" dxfId="0" priority="118" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE22">
+    <cfRule type="cellIs" dxfId="0" priority="120" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE23">
+    <cfRule type="cellIs" dxfId="0" priority="122" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE8">
+    <cfRule type="cellIs" dxfId="0" priority="94" operator="lessThanOrEqual">
+      <formula>I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE9">
+    <cfRule type="cellIs" dxfId="0" priority="96" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ11">
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ12">
+    <cfRule type="cellIs" dxfId="0" priority="127" operator="lessThanOrEqual">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ14">
+    <cfRule type="cellIs" dxfId="0" priority="129" operator="lessThanOrEqual">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ15">
+    <cfRule type="cellIs" dxfId="0" priority="131" operator="lessThanOrEqual">
       <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD16">
-    <cfRule type="cellIs" dxfId="0" priority="95" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AJ16">
+    <cfRule type="cellIs" dxfId="0" priority="133" operator="lessThanOrEqual">
       <formula>H16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD18">
-    <cfRule type="cellIs" dxfId="0" priority="97" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AJ17">
+    <cfRule type="cellIs" dxfId="0" priority="135" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ18">
+    <cfRule type="cellIs" dxfId="0" priority="137" operator="lessThanOrEqual">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD19">
-    <cfRule type="cellIs" dxfId="0" priority="99" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AJ19">
+    <cfRule type="cellIs" dxfId="0" priority="139" operator="lessThanOrEqual">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD20">
-    <cfRule type="cellIs" dxfId="0" priority="101" operator="lessThanOrEqual">
-      <formula>H20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD22">
-    <cfRule type="cellIs" dxfId="0" priority="103" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AJ22">
+    <cfRule type="cellIs" dxfId="0" priority="141" operator="lessThanOrEqual">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD23">
-    <cfRule type="cellIs" dxfId="0" priority="105" operator="lessThanOrEqual">
-      <formula>H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD8">
-    <cfRule type="cellIs" dxfId="0" priority="81" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AJ8">
+    <cfRule type="cellIs" dxfId="0" priority="123" operator="lessThanOrEqual">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD9">
-    <cfRule type="cellIs" dxfId="0" priority="83" operator="lessThanOrEqual">
-      <formula>H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE10">
-    <cfRule type="cellIs" dxfId="0" priority="86" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE11">
-    <cfRule type="cellIs" dxfId="0" priority="88" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK11">
+    <cfRule type="cellIs" dxfId="0" priority="126" operator="lessThanOrEqual">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE13">
-    <cfRule type="cellIs" dxfId="0" priority="90" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE14">
-    <cfRule type="cellIs" dxfId="0" priority="92" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK12">
+    <cfRule type="cellIs" dxfId="0" priority="128" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK14">
+    <cfRule type="cellIs" dxfId="0" priority="130" operator="lessThanOrEqual">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE15">
-    <cfRule type="cellIs" dxfId="0" priority="94" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK15">
+    <cfRule type="cellIs" dxfId="0" priority="132" operator="lessThanOrEqual">
       <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE16">
-    <cfRule type="cellIs" dxfId="0" priority="96" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK16">
+    <cfRule type="cellIs" dxfId="0" priority="134" operator="lessThanOrEqual">
       <formula>I16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE18">
-    <cfRule type="cellIs" dxfId="0" priority="98" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK17">
+    <cfRule type="cellIs" dxfId="0" priority="136" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK18">
+    <cfRule type="cellIs" dxfId="0" priority="138" operator="lessThanOrEqual">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE19">
-    <cfRule type="cellIs" dxfId="0" priority="100" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK19">
+    <cfRule type="cellIs" dxfId="0" priority="140" operator="lessThanOrEqual">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE20">
-    <cfRule type="cellIs" dxfId="0" priority="102" operator="lessThanOrEqual">
-      <formula>I20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE22">
-    <cfRule type="cellIs" dxfId="0" priority="104" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AK22">
+    <cfRule type="cellIs" dxfId="0" priority="142" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE23">
-    <cfRule type="cellIs" dxfId="0" priority="106" operator="lessThanOrEqual">
-      <formula>I23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE8">
-    <cfRule type="cellIs" dxfId="0" priority="82" operator="lessThanOrEqual">
-      <formula>I8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE9">
-    <cfRule type="cellIs" dxfId="0" priority="84" operator="lessThanOrEqual">
-      <formula>I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11">
-    <cfRule type="cellIs" dxfId="0" priority="109" operator="lessThanOrEqual">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ12">
-    <cfRule type="cellIs" dxfId="0" priority="111" operator="lessThanOrEqual">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ14">
-    <cfRule type="cellIs" dxfId="0" priority="113" operator="lessThanOrEqual">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15">
-    <cfRule type="cellIs" dxfId="0" priority="115" operator="lessThanOrEqual">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ16">
-    <cfRule type="cellIs" dxfId="0" priority="117" operator="lessThanOrEqual">
-      <formula>H16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="0" priority="119" operator="lessThanOrEqual">
-      <formula>H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="0" priority="121" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ22">
-    <cfRule type="cellIs" dxfId="0" priority="123" operator="lessThanOrEqual">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ8">
-    <cfRule type="cellIs" dxfId="0" priority="107" operator="lessThanOrEqual">
-      <formula>H8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK11">
-    <cfRule type="cellIs" dxfId="0" priority="110" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK12">
-    <cfRule type="cellIs" dxfId="0" priority="112" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK14">
-    <cfRule type="cellIs" dxfId="0" priority="114" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK15">
-    <cfRule type="cellIs" dxfId="0" priority="116" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK16">
-    <cfRule type="cellIs" dxfId="0" priority="118" operator="lessThanOrEqual">
-      <formula>I16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK18">
-    <cfRule type="cellIs" dxfId="0" priority="120" operator="lessThanOrEqual">
-      <formula>I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK19">
-    <cfRule type="cellIs" dxfId="0" priority="122" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK22">
+  <conditionalFormatting sqref="AK8">
     <cfRule type="cellIs" dxfId="0" priority="124" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK8">
-    <cfRule type="cellIs" dxfId="0" priority="108" operator="lessThanOrEqual">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4914,23 +5094,33 @@
       <formula>H16</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R17">
+    <cfRule type="cellIs" dxfId="0" priority="47" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R18">
-    <cfRule type="cellIs" dxfId="0" priority="47" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="lessThanOrEqual">
       <formula>H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19">
-    <cfRule type="cellIs" dxfId="0" priority="49" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="lessThanOrEqual">
       <formula>H19</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R21">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="lessThanOrEqual">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="cellIs" dxfId="0" priority="51" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="55" operator="lessThanOrEqual">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23">
-    <cfRule type="cellIs" dxfId="0" priority="53" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="lessThanOrEqual">
       <formula>H23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4964,23 +5154,33 @@
       <formula>I16</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S17">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="0" priority="48" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="50" operator="lessThanOrEqual">
       <formula>I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19">
-    <cfRule type="cellIs" dxfId="0" priority="50" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="lessThanOrEqual">
       <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S21">
+    <cfRule type="cellIs" dxfId="0" priority="54" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="cellIs" dxfId="0" priority="52" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="56" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S23">
-    <cfRule type="cellIs" dxfId="0" priority="54" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="lessThanOrEqual">
       <formula>I23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4995,132 +5195,172 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X10">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="lessThanOrEqual">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X11">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X12">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="lessThanOrEqual">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X13">
+    <cfRule type="cellIs" dxfId="0" priority="71" operator="lessThanOrEqual">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X14">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="lessThanOrEqual">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X15">
+    <cfRule type="cellIs" dxfId="0" priority="75" operator="lessThanOrEqual">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X16">
+    <cfRule type="cellIs" dxfId="0" priority="77" operator="lessThanOrEqual">
+      <formula>H16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17">
+    <cfRule type="cellIs" dxfId="0" priority="79" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X18">
+    <cfRule type="cellIs" dxfId="0" priority="81" operator="lessThanOrEqual">
+      <formula>H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X19">
+    <cfRule type="cellIs" dxfId="0" priority="83" operator="lessThanOrEqual">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X20">
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="lessThanOrEqual">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X21">
+    <cfRule type="cellIs" dxfId="0" priority="87" operator="lessThanOrEqual">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X22">
+    <cfRule type="cellIs" dxfId="0" priority="89" operator="lessThanOrEqual">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X23">
+    <cfRule type="cellIs" dxfId="0" priority="91" operator="lessThanOrEqual">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X7">
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="lessThanOrEqual">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X8">
     <cfRule type="cellIs" dxfId="0" priority="61" operator="lessThanOrEqual">
-      <formula>H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X12">
+      <formula>H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X9">
     <cfRule type="cellIs" dxfId="0" priority="63" operator="lessThanOrEqual">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X14">
-    <cfRule type="cellIs" dxfId="0" priority="65" operator="lessThanOrEqual">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X15">
-    <cfRule type="cellIs" dxfId="0" priority="67" operator="lessThanOrEqual">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X16">
-    <cfRule type="cellIs" dxfId="0" priority="69" operator="lessThanOrEqual">
-      <formula>H16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X18">
-    <cfRule type="cellIs" dxfId="0" priority="71" operator="lessThanOrEqual">
-      <formula>H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X19">
-    <cfRule type="cellIs" dxfId="0" priority="73" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X20">
-    <cfRule type="cellIs" dxfId="0" priority="75" operator="lessThanOrEqual">
-      <formula>H20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X22">
-    <cfRule type="cellIs" dxfId="0" priority="77" operator="lessThanOrEqual">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X23">
-    <cfRule type="cellIs" dxfId="0" priority="79" operator="lessThanOrEqual">
-      <formula>H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X7">
-    <cfRule type="cellIs" dxfId="0" priority="55" operator="lessThanOrEqual">
-      <formula>H7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X8">
-    <cfRule type="cellIs" dxfId="0" priority="57" operator="lessThanOrEqual">
-      <formula>H8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X9">
-    <cfRule type="cellIs" dxfId="0" priority="59" operator="lessThanOrEqual">
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10">
+    <cfRule type="cellIs" dxfId="0" priority="66" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" dxfId="0" priority="68" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y12">
+    <cfRule type="cellIs" dxfId="0" priority="70" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y13">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y14">
+    <cfRule type="cellIs" dxfId="0" priority="74" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y15">
+    <cfRule type="cellIs" dxfId="0" priority="76" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y16">
+    <cfRule type="cellIs" dxfId="0" priority="78" operator="lessThanOrEqual">
+      <formula>I16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y17">
+    <cfRule type="cellIs" dxfId="0" priority="80" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y18">
+    <cfRule type="cellIs" dxfId="0" priority="82" operator="lessThanOrEqual">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y19">
+    <cfRule type="cellIs" dxfId="0" priority="84" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y20">
+    <cfRule type="cellIs" dxfId="0" priority="86" operator="lessThanOrEqual">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y21">
+    <cfRule type="cellIs" dxfId="0" priority="88" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y22">
+    <cfRule type="cellIs" dxfId="0" priority="90" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y23">
+    <cfRule type="cellIs" dxfId="0" priority="92" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y7">
+    <cfRule type="cellIs" dxfId="0" priority="60" operator="lessThanOrEqual">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y8">
     <cfRule type="cellIs" dxfId="0" priority="62" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y12">
+      <formula>I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y9">
     <cfRule type="cellIs" dxfId="0" priority="64" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y14">
-    <cfRule type="cellIs" dxfId="0" priority="66" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y15">
-    <cfRule type="cellIs" dxfId="0" priority="68" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y16">
-    <cfRule type="cellIs" dxfId="0" priority="70" operator="lessThanOrEqual">
-      <formula>I16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y18">
-    <cfRule type="cellIs" dxfId="0" priority="72" operator="lessThanOrEqual">
-      <formula>I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y19">
-    <cfRule type="cellIs" dxfId="0" priority="74" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y20">
-    <cfRule type="cellIs" dxfId="0" priority="76" operator="lessThanOrEqual">
-      <formula>I20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y22">
-    <cfRule type="cellIs" dxfId="0" priority="78" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y23">
-    <cfRule type="cellIs" dxfId="0" priority="80" operator="lessThanOrEqual">
-      <formula>I23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y7">
-    <cfRule type="cellIs" dxfId="0" priority="56" operator="lessThanOrEqual">
-      <formula>I7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y8">
-    <cfRule type="cellIs" dxfId="0" priority="58" operator="lessThanOrEqual">
-      <formula>I8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y9">
-    <cfRule type="cellIs" dxfId="0" priority="60" operator="lessThanOrEqual">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5168,31 +5408,38 @@
     <hyperlink ref="AG16" r:id="rId41"/>
     <hyperlink ref="AM16" r:id="rId42"/>
     <hyperlink ref="O17" r:id="rId43"/>
-    <hyperlink ref="O18" r:id="rId44"/>
-    <hyperlink ref="U18" r:id="rId45"/>
-    <hyperlink ref="AA18" r:id="rId46"/>
-    <hyperlink ref="AG18" r:id="rId47"/>
-    <hyperlink ref="AM18" r:id="rId48"/>
-    <hyperlink ref="O19" r:id="rId49"/>
-    <hyperlink ref="U19" r:id="rId50"/>
-    <hyperlink ref="AA19" r:id="rId51"/>
-    <hyperlink ref="AG19" r:id="rId52"/>
-    <hyperlink ref="AM19" r:id="rId53"/>
-    <hyperlink ref="O20" r:id="rId54"/>
-    <hyperlink ref="AA20" r:id="rId55"/>
-    <hyperlink ref="AG20" r:id="rId56"/>
-    <hyperlink ref="O21" r:id="rId57"/>
-    <hyperlink ref="O22" r:id="rId58"/>
-    <hyperlink ref="U22" r:id="rId59"/>
-    <hyperlink ref="AA22" r:id="rId60"/>
-    <hyperlink ref="AG22" r:id="rId61"/>
-    <hyperlink ref="AM22" r:id="rId62"/>
-    <hyperlink ref="O23" r:id="rId63"/>
-    <hyperlink ref="U23" r:id="rId64"/>
-    <hyperlink ref="AA23" r:id="rId65"/>
-    <hyperlink ref="AG23" r:id="rId66"/>
+    <hyperlink ref="U17" r:id="rId44"/>
+    <hyperlink ref="AA17" r:id="rId45"/>
+    <hyperlink ref="AG17" r:id="rId46"/>
+    <hyperlink ref="AM17" r:id="rId47"/>
+    <hyperlink ref="O18" r:id="rId48"/>
+    <hyperlink ref="U18" r:id="rId49"/>
+    <hyperlink ref="AA18" r:id="rId50"/>
+    <hyperlink ref="AG18" r:id="rId51"/>
+    <hyperlink ref="AM18" r:id="rId52"/>
+    <hyperlink ref="O19" r:id="rId53"/>
+    <hyperlink ref="U19" r:id="rId54"/>
+    <hyperlink ref="AA19" r:id="rId55"/>
+    <hyperlink ref="AG19" r:id="rId56"/>
+    <hyperlink ref="AM19" r:id="rId57"/>
+    <hyperlink ref="O20" r:id="rId58"/>
+    <hyperlink ref="AA20" r:id="rId59"/>
+    <hyperlink ref="AG20" r:id="rId60"/>
+    <hyperlink ref="O21" r:id="rId61"/>
+    <hyperlink ref="U21" r:id="rId62"/>
+    <hyperlink ref="AA21" r:id="rId63"/>
+    <hyperlink ref="AG21" r:id="rId64"/>
+    <hyperlink ref="O22" r:id="rId65"/>
+    <hyperlink ref="U22" r:id="rId66"/>
+    <hyperlink ref="AA22" r:id="rId67"/>
+    <hyperlink ref="AG22" r:id="rId68"/>
+    <hyperlink ref="AM22" r:id="rId69"/>
+    <hyperlink ref="O23" r:id="rId70"/>
+    <hyperlink ref="U23" r:id="rId71"/>
+    <hyperlink ref="AA23" r:id="rId72"/>
+    <hyperlink ref="AG23" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId67"/>
+  <legacyDrawing r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se mejora el pcb y la vist 3d. Se actualizan los costos con kicost. Se agrega tutorial FreeRouting
</commit_message>
<xml_diff>
--- a/PonchoEDUCIAA_WIFI_BLT.xlsx
+++ b/PonchoEDUCIAA_WIFI_BLT.xlsx
@@ -7,17 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="PonchoEDUCIAA_WIFI_BLT" sheetId="1" r:id="rId1"/>
+    <sheet name="PonchoEDUCIAA_WIFI_BLT2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty">'PonchoEDUCIAA_WIFI_BLT'!$I$1</definedName>
-    <definedName name="digikey_part_data">'PonchoEDUCIAA_WIFI_BLT'!$J$5:$O$24</definedName>
-    <definedName name="farnell_part_data">'PonchoEDUCIAA_WIFI_BLT'!$P$5:$U$24</definedName>
-    <definedName name="global_part_data">'PonchoEDUCIAA_WIFI_BLT'!$A$5:$I$24</definedName>
-    <definedName name="mouser_part_data">'PonchoEDUCIAA_WIFI_BLT'!$V$5:$AA$24</definedName>
-    <definedName name="newark_part_data">'PonchoEDUCIAA_WIFI_BLT'!$AB$5:$AG$24</definedName>
-    <definedName name="rs_part_data">'PonchoEDUCIAA_WIFI_BLT'!$AH$5:$AM$24</definedName>
-    <definedName name="TotalCost">'PonchoEDUCIAA_WIFI_BLT'!$I$2</definedName>
+    <definedName name="BoardQty">'PonchoEDUCIAA_WIFI_BLT2'!$I$1</definedName>
+    <definedName name="digikey_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$J$5:$O$24</definedName>
+    <definedName name="farnell_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$P$5:$U$24</definedName>
+    <definedName name="global_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$A$5:$I$24</definedName>
+    <definedName name="mouser_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$V$5:$AA$24</definedName>
+    <definedName name="newark_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$AB$5:$AG$24</definedName>
+    <definedName name="rs_part_data">'PonchoEDUCIAA_WIFI_BLT2'!$AH$5:$AM$24</definedName>
+    <definedName name="TotalCost">'PonchoEDUCIAA_WIFI_BLT2'!$I$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="182">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -633,16 +633,16 @@
     <t>LED_Verde</t>
   </si>
   <si>
-    <t>LED 5MM VERT HE DIFF GRN PC MNT</t>
-  </si>
-  <si>
-    <t>LEDs:LED_0402</t>
-  </si>
-  <si>
-    <t>Dialight</t>
-  </si>
-  <si>
-    <t>5612201050F</t>
+    <t>LED GREEN DIFFUSED 0805 SMD</t>
+  </si>
+  <si>
+    <t>LEDs:LED_0805</t>
+  </si>
+  <si>
+    <t>OSRAM Opto Semiconductors Inc.</t>
+  </si>
+  <si>
+    <t>LG R971-KN-1</t>
   </si>
   <si>
     <t>D3</t>
@@ -651,10 +651,10 @@
     <t>LED_Amarillo</t>
   </si>
   <si>
-    <t>LED 5MM 5V VERTICAL YELLOW PCMNT</t>
-  </si>
-  <si>
-    <t>5500804F</t>
+    <t>LED YELLOW DIFFUSED 0805 SMD</t>
+  </si>
+  <si>
+    <t>LY R976-PS-36</t>
   </si>
   <si>
     <t>D1</t>
@@ -663,10 +663,10 @@
     <t>LED_Rojo</t>
   </si>
   <si>
-    <t>LED 5MM 5V VERTICAL RED PC MNT</t>
-  </si>
-  <si>
-    <t>5500504F</t>
+    <t>LED RED DIFFUSED 0805 SMD</t>
+  </si>
+  <si>
+    <t>LS R976-NR-1</t>
   </si>
   <si>
     <t>J1</t>
@@ -873,13 +873,13 @@
     <t>311-402CRCT-ND</t>
   </si>
   <si>
-    <t>350-2814-ND</t>
-  </si>
-  <si>
-    <t>350-1615-ND</t>
-  </si>
-  <si>
-    <t>350-1608-ND</t>
+    <t>475-1410-1-ND</t>
+  </si>
+  <si>
+    <t>475-2560-1-ND</t>
+  </si>
+  <si>
+    <t>475-1278-1-ND</t>
   </si>
   <si>
     <t>WM4112-ND</t>
@@ -918,7 +918,7 @@
     <t>Farnell</t>
   </si>
   <si>
-    <t>1654365</t>
+    <t>1654363</t>
   </si>
   <si>
     <t>1022306</t>
@@ -966,13 +966,13 @@
     <t>603-RC0805FR-07402RL</t>
   </si>
   <si>
-    <t>645-561-2201-050F</t>
-  </si>
-  <si>
-    <t>645-550-0804F</t>
-  </si>
-  <si>
-    <t>645-550-0504F</t>
+    <t>720-LGR971-KN-1</t>
+  </si>
+  <si>
+    <t>720-LYR976-PS-36</t>
+  </si>
+  <si>
+    <t>720-LSR976-NR-1</t>
   </si>
   <si>
     <t>538-22-27-2031</t>
@@ -1020,25 +1020,19 @@
     <t>66R3296</t>
   </si>
   <si>
-    <t>30K3275</t>
-  </si>
-  <si>
-    <t>87M2237</t>
-  </si>
-  <si>
     <t>13T6895</t>
   </si>
   <si>
-    <t>03AC2607</t>
-  </si>
-  <si>
-    <t>03AC2742</t>
+    <t>48W5738</t>
+  </si>
+  <si>
+    <t>13T1205</t>
   </si>
   <si>
     <t>85K9474</t>
   </si>
   <si>
-    <t>89K7298</t>
+    <t>68X3202</t>
   </si>
   <si>
     <t>08N2142</t>
@@ -1068,10 +1062,7 @@
     <t>681-1193</t>
   </si>
   <si>
-    <t>546-0700</t>
-  </si>
-  <si>
-    <t>546-0687</t>
+    <t>418-044</t>
   </si>
   <si>
     <t>723-5363</t>
@@ -1090,6 +1081,9 @@
   </si>
   <si>
     <t>776-9194</t>
+  </si>
+  <si>
+    <t>136-4985</t>
   </si>
   <si>
     <t>102-327</t>
@@ -1700,7 +1694,7 @@
       <c r="AF5" s="10"/>
       <c r="AG5" s="10"/>
       <c r="AH5" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AI5" s="11"/>
       <c r="AJ5" s="11"/>
@@ -1876,7 +1870,7 @@
         <v>106</v>
       </c>
       <c r="R7" s="13">
-        <f>iferror(lookup(if(Q7="",G7,Q7),{0,1,5,15,25,75,150,250,500},{0.0,1.7752099999999997,1.62639,1.4775699999999998,1.43505,1.39253,1.35001,1.33938,1.31812}),"")</f>
+        <f>iferror(lookup(if(Q7="",G7,Q7),{0,1,10,50,100,500},{0.0,1.62639,1.35001,1.2755999999999998,1.23308,1.21182}),"")</f>
         <v>0</v>
       </c>
       <c r="S7" s="13">
@@ -1890,10 +1884,10 @@
         <v>106</v>
       </c>
       <c r="V7">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="X7" s="13">
-        <f>iferror(lookup(if(W7="",G7,W7),{0,1,10},{0.0,8.97,8.08}),"")</f>
+        <f>iferror(lookup(if(W7="",G7,W7),{0,1},{0.0,8.98}),"")</f>
         <v>0</v>
       </c>
       <c r="Y7" s="13">
@@ -1916,7 +1910,7 @@
         <v>60</v>
       </c>
       <c r="AL7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AM7" s="14" t="s">
         <v>106</v>
@@ -1954,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>2552</v>
+        <v>2297</v>
       </c>
       <c r="L8" s="13">
         <f>iferror(lookup(if(K8="",G8,K8),{0,1,10,100,500,1000,5000,10000},{0.0,2.0,1.815,1.5561,1.29676,1.1115,0.98553,0.9633}),"")</f>
@@ -1985,10 +1979,10 @@
         <v>106</v>
       </c>
       <c r="V8">
-        <v>3558</v>
+        <v>3483</v>
       </c>
       <c r="X8" s="13">
-        <f>iferror(lookup(if(W8="",G8,W8),{0,1,10,100,250,500,1000},{0.0,2.0,1.64,1.56,1.4,1.29,1.21}),"")</f>
+        <f>iferror(lookup(if(W8="",G8,W8),{0,1,10,100,250,500,1000},{0.0,2.01,1.64,1.56,1.4,1.3,1.27}),"")</f>
         <v>0</v>
       </c>
       <c r="Y8" s="13">
@@ -2027,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="AL8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AM8" s="14" t="s">
         <v>106</v>
@@ -2065,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>101602</v>
+        <v>161830</v>
       </c>
       <c r="L9" s="13">
         <f>iferror(lookup(if(K9="",G9,K9),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0.0,0.1,0.022,0.0088,0.00396,0.00344,0.00284,0.00247,0.00217,0.00199,0.00195}),"")</f>
@@ -2082,10 +2076,10 @@
         <v>106</v>
       </c>
       <c r="V9">
-        <v>47564</v>
+        <v>47264</v>
       </c>
       <c r="X9" s="13">
-        <f>iferror(lookup(if(W9="",G9,W9),{0,1,10,100,1000,5000,25000},{0.0,0.101,0.016,0.006,0.004,0.003,0.002}),"")</f>
+        <f>iferror(lookup(if(W9="",G9,W9),{0,1,10,100,1000,5000,25000},{0.0,0.1,0.017,0.006,0.004,0.004,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y9" s="13">
@@ -2145,10 +2139,10 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>561662</v>
       </c>
       <c r="L10" s="13">
-        <f>iferror(lookup(if(K10="",G10,K10),{0,1,10,25,100,250,500,1000,2500,5000},{0.0,1.24,1.004,0.7724,0.6953,0.618,0.5253,0.4326,0.41097,0.4017}),"")</f>
+        <f>iferror(lookup(if(K10="",G10,K10),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000},{0.0,0.25,0.18,0.1328,0.0948,0.06448,0.0569,0.04457,0.03966,0.03449,0.03104,0.02874}),"")</f>
         <v>0</v>
       </c>
       <c r="M10" s="13">
@@ -2162,10 +2156,10 @@
         <v>106</v>
       </c>
       <c r="V10">
-        <v>1010</v>
+        <v>330836</v>
       </c>
       <c r="X10" s="13">
-        <f>iferror(lookup(if(W10="",G10,W10),{0,1,10,100,500,1000,2500,5000},{0.0,1.23,0.775,0.619,0.526,0.435,0.412,0.403}),"")</f>
+        <f>iferror(lookup(if(W10="",G10,W10),{0,1,10,100,500,1000,2000,4000,8000},{0.0,0.231,0.164,0.07,0.059,0.045,0.04,0.034,0.031}),"")</f>
         <v>0</v>
       </c>
       <c r="Y10" s="13">
@@ -2178,18 +2172,21 @@
       <c r="AA10" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AD10" s="13">
-        <f>iferror(lookup(if(AC10="",G10,AC10),{0,1,1625},{0.0,0.433,0.433}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AE10" s="13">
-        <f>iferror(if(AC10="",G10,AC10)*AD10,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG10" s="14" t="s">
+      <c r="AH10">
+        <v>26300</v>
+      </c>
+      <c r="AJ10" s="13">
+        <f>iferror(lookup(if(AI10="",G10,AI10),{0,1,50,500},{0.0,0.09885899999999999,0.09885899999999999,0.082914}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK10" s="13">
+        <f>iferror(if(AI10="",G10,AI10)*AJ10,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>173</v>
+      </c>
+      <c r="AM10" s="14" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2225,10 +2222,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>1173</v>
+        <v>245886</v>
       </c>
       <c r="L11" s="13">
-        <f>iferror(lookup(if(K11="",G11,K11),{0,1,10,25,100,250,500,1000,2500,5000},{0.0,1.75,1.42,1.0924,0.9833,0.874,0.7429,0.6118,0.58121,0.5681}),"")</f>
+        <f>iferror(lookup(if(K11="",G11,K11),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0.0,0.35,0.253,0.1864,0.1331,0.09052,0.07986,0.06256,0.05566,0.0484,0.04356,0.03872,0.03267}),"")</f>
         <v>0</v>
       </c>
       <c r="M11" s="13">
@@ -2242,10 +2239,10 @@
         <v>106</v>
       </c>
       <c r="V11">
-        <v>340</v>
+        <v>66042</v>
       </c>
       <c r="X11" s="13">
-        <f>iferror(lookup(if(W11="",G11,W11),{0,1,10,100,500,1000,2500,5000},{0.0,1.76,1.09,0.876,0.745,0.614,0.582,0.569}),"")</f>
+        <f>iferror(lookup(if(W11="",G11,W11),{0,1,10,100,500,1000,2000,4000,8000},{0.0,0.251,0.172,0.072,0.063,0.055,0.042,0.037,0.033}),"")</f>
         <v>0</v>
       </c>
       <c r="Y11" s="13">
@@ -2256,37 +2253,6 @@
         <v>142</v>
       </c>
       <c r="AA11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD11" s="13">
-        <f>iferror(lookup(if(AC11="",G11,AC11),{0,1,10,25,50,100,250,500,1000},{0.0,1.75,1.09,1.02,0.946,0.874,0.809,0.743,0.612}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="13">
-        <f>iferror(if(AC11="",G11,AC11)*AD11,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG11" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH11">
-        <v>57</v>
-      </c>
-      <c r="AJ11" s="13">
-        <f>iferror(lookup(if(AI11="",G11,AI11),{0,1,25,100,250,500},{0.0,1.3606399999999998,0.8504,0.69095,0.6271699999999999,0.57402}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AK11" s="13">
-        <f>iferror(if(AI11="",G11,AI11)*AJ11,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>175</v>
-      </c>
-      <c r="AM11" s="14" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2322,10 +2288,10 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>992</v>
+        <v>283564</v>
       </c>
       <c r="L12" s="13">
-        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500},{0.0,1.75,1.42,1.0924,0.9833,0.874,0.7429}),"")</f>
+        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000},{0.0,0.26,0.19,0.1396,0.0998,0.06788,0.0599,0.04692,0.04175,0.0363,0.03267,0.03025}),"")</f>
         <v>0</v>
       </c>
       <c r="M12" s="13">
@@ -2339,10 +2305,10 @@
         <v>106</v>
       </c>
       <c r="V12">
-        <v>79</v>
+        <v>295516</v>
       </c>
       <c r="X12" s="13">
-        <f>iferror(lookup(if(W12="",G12,W12),{0,1,10,100,500,1000,2500,5000},{0.0,1.76,1.09,0.876,0.745,0.614,0.582,0.569}),"")</f>
+        <f>iferror(lookup(if(W12="",G12,W12),{0,1,10,100,500,1000,2000,4000,8000,24000},{0.0,0.261,0.14,0.068,0.06,0.047,0.042,0.037,0.033,0.032}),"")</f>
         <v>0</v>
       </c>
       <c r="Y12" s="13">
@@ -2353,23 +2319,6 @@
         <v>143</v>
       </c>
       <c r="AA12" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH12">
-        <v>22</v>
-      </c>
-      <c r="AJ12" s="13">
-        <f>iferror(lookup(if(AI12="",G12,AI12),{0,1,25,100,250,500},{0.0,1.2437099999999999,0.77599,0.6271699999999999,0.58465,0.5315}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AK12" s="13">
-        <f>iferror(if(AI12="",G12,AI12)*AJ12,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>176</v>
-      </c>
-      <c r="AM12" s="14" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2405,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>48007</v>
+        <v>42438</v>
       </c>
       <c r="L13" s="13">
         <f>iferror(lookup(if(K13="",G13,K13),{0,1,10,25,50,100,250,500,1000,2500},{0.0,0.35,0.334,0.2864,0.2436,0.234,0.21012,0.20056,0.16713,0.1528}),"")</f>
@@ -2436,10 +2385,10 @@
         <v>106</v>
       </c>
       <c r="V13">
-        <v>25266</v>
+        <v>23619</v>
       </c>
       <c r="X13" s="13">
-        <f>iferror(lookup(if(W13="",G13,W13),{0,1,10,100,500,1000,2500,10000,25000,50000},{0.0,0.361,0.269,0.233,0.202,0.168,0.153,0.134,0.129,0.125}),"")</f>
+        <f>iferror(lookup(if(W13="",G13,W13),{0,1,10,100,500,1000,2500,10000,25000,50000},{0.0,0.361,0.269,0.232,0.202,0.169,0.153,0.135,0.13,0.125}),"")</f>
         <v>0</v>
       </c>
       <c r="Y13" s="13">
@@ -2461,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AG13" s="14" t="s">
         <v>106</v>
@@ -2499,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1848285</v>
+        <v>3103986</v>
       </c>
       <c r="L14" s="13">
         <f>iferror(lookup(if(K14="",G14,K14),{0,1,10,100,500,1000,2500,5000,10000,20000,30000},{0.0,0.1,0.014,0.0062,0.00442,0.00348,0.00316,0.00291,0.00231,0.0022,0.00209}),"")</f>
@@ -2530,10 +2479,10 @@
         <v>106</v>
       </c>
       <c r="V14">
-        <v>689964</v>
+        <v>680207</v>
       </c>
       <c r="X14" s="13">
-        <f>iferror(lookup(if(W14="",G14,W14),{0,1,10,100,500,2500,10000},{0.0,0.101,0.006,0.004,0.003,0.002,0.002}),"")</f>
+        <f>iferror(lookup(if(W14="",G14,W14),{0,1,10,100,2500,10000},{0.0,0.1,0.006,0.004,0.002,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y14" s="13">
@@ -2547,7 +2496,7 @@
         <v>106</v>
       </c>
       <c r="AD14" s="13">
-        <f>iferror(lookup(if(AC14="",G14,AC14),{0,1,10000,20000},{0.0,0.003,0.003,0.003}),"")</f>
+        <f>iferror(lookup(if(AC14="",G14,AC14),{0,1,10,25,50,100,250,500},{0.0,0.006,0.006,0.005,0.005,0.004,0.004,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AE14" s="13">
@@ -2555,13 +2504,13 @@
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AG14" s="14" t="s">
         <v>106</v>
       </c>
       <c r="AH14">
-        <v>1600</v>
+        <v>600</v>
       </c>
       <c r="AJ14" s="13">
         <f>iferror(lookup(if(AI14="",G14,AI14),{0,1,200,1000},{0.0,0.006378,0.006378,0.004252}),"")</f>
@@ -2572,7 +2521,7 @@
         <v>0</v>
       </c>
       <c r="AL14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AM14" s="14" t="s">
         <v>106</v>
@@ -2610,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>616770</v>
+        <v>493075</v>
       </c>
       <c r="L15" s="13">
         <f>iferror(lookup(if(K15="",G15,K15),{0,1,10,100,500,1000,4000,8000,12000},{0.0,0.15,0.105,0.0495,0.03472,0.02875,0.02129,0.0198,0.01881}),"")</f>
@@ -2641,10 +2590,10 @@
         <v>106</v>
       </c>
       <c r="V15">
-        <v>52280</v>
+        <v>47930</v>
       </c>
       <c r="X15" s="13">
-        <f>iferror(lookup(if(W15="",G15,W15),{0,1,10,100,500,1000,4000},{0.0,0.241,0.113,0.064,0.057,0.048,0.036}),"")</f>
+        <f>iferror(lookup(if(W15="",G15,W15),{0,1,10,100,500,1000,4000},{0.0,0.241,0.113,0.064,0.057,0.048,0.037}),"")</f>
         <v>0</v>
       </c>
       <c r="Y15" s="13">
@@ -2658,7 +2607,7 @@
         <v>106</v>
       </c>
       <c r="AD15" s="13">
-        <f>iferror(lookup(if(AC15="",G15,AC15),{0,1,4000,8000,16000,24000,40000},{0.0,0.051,0.051,0.047,0.044,0.042,0.042}),"")</f>
+        <f>iferror(lookup(if(AC15="",G15,AC15),{0,1,10,25,50,100,250,500,1000},{0.0,0.113,0.113,0.097,0.08,0.064,0.061,0.057,0.048}),"")</f>
         <v>0</v>
       </c>
       <c r="AE15" s="13">
@@ -2666,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AG15" s="14" t="s">
         <v>106</v>
@@ -2683,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="AL15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AM15" s="14" t="s">
         <v>106</v>
@@ -2720,9 +2669,6 @@
         <f>iferror(G16*H16,"")</f>
         <v>0</v>
       </c>
-      <c r="J16">
-        <v>117</v>
-      </c>
       <c r="L16" s="13">
         <f>iferror(lookup(if(K16="",G16,K16),{0,1,10,100,500,1000,2500,5000,15000,30000},{0.0,0.1,0.011,0.005,0.00354,0.00278,0.00253,0.00233,0.00176,0.00167}),"")</f>
         <v>0</v>
@@ -2752,10 +2698,10 @@
         <v>106</v>
       </c>
       <c r="V16">
-        <v>6348</v>
+        <v>724180</v>
       </c>
       <c r="X16" s="13">
-        <f>iferror(lookup(if(W16="",G16,W16),{0,1,100,1000,15000},{0.0,0.101,0.039,0.024,0.002}),"")</f>
+        <f>iferror(lookup(if(W16="",G16,W16),{0,1,100,1000,15000},{0.0,0.1,0.039,0.024,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y16" s="13">
@@ -2777,13 +2723,13 @@
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AG16" s="14" t="s">
         <v>106</v>
       </c>
       <c r="AH16">
-        <v>13100</v>
+        <v>26500</v>
       </c>
       <c r="AJ16" s="13">
         <f>iferror(lookup(if(AI16="",G16,AI16),{0,1,100,1000},{0.0,0.052087,0.052087,0.030827}),"")</f>
@@ -2794,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="AL16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AM16" s="14" t="s">
         <v>106</v>
@@ -2832,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>1202983</v>
+        <v>1082937</v>
       </c>
       <c r="L17" s="13">
         <f>iferror(lookup(if(K17="",G17,K17),{0,1,10,100,1000,2500,5000,10000,25000,50000,125000},{0.0,0.1,0.022,0.0088,0.00396,0.00344,0.00284,0.00247,0.00217,0.00199,0.00195}),"")</f>
@@ -2863,10 +2809,10 @@
         <v>106</v>
       </c>
       <c r="V17">
-        <v>66451</v>
+        <v>197970</v>
       </c>
       <c r="X17" s="13">
-        <f>iferror(lookup(if(W17="",G17,W17),{0,1,10,100,1000,5000,25000},{0.0,0.101,0.016,0.006,0.004,0.003,0.002}),"")</f>
+        <f>iferror(lookup(if(W17="",G17,W17),{0,1,10,100,1000,5000,25000},{0.0,0.1,0.017,0.006,0.004,0.004,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y17" s="13">
@@ -2880,7 +2826,7 @@
         <v>106</v>
       </c>
       <c r="AD17" s="13">
-        <f>iferror(lookup(if(AC17="",G17,AC17),{0,1,10,25,100,250,1000},{0.0,0.026,0.026,0.018,0.011,0.008,0.006}),"")</f>
+        <f>iferror(lookup(if(AC17="",G17,AC17),{0,1,5000,10000,25000},{0.0,0.003,0.003,0.002,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="AE17" s="13">
@@ -2888,13 +2834,13 @@
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AG17" s="14" t="s">
         <v>106</v>
       </c>
       <c r="AH17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AJ17" s="13">
         <f>iferror(lookup(if(AI17="",G17,AI17),{0,1,5},{0.0,23.364739999999998,19.293449999999996}),"")</f>
@@ -2905,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="AL17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AM17" s="14" t="s">
         <v>106</v>
@@ -2943,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>540440</v>
+        <v>461074</v>
       </c>
       <c r="L18" s="13">
         <f>iferror(lookup(if(K18="",G18,K18),{0,1,10,100,1000,2500,5000,10000,25000},{0.0,0.36,0.302,0.1182,0.04948,0.04536,0.03749,0.03499,0.03451}),"")</f>
@@ -2974,10 +2920,10 @@
         <v>106</v>
       </c>
       <c r="V18">
-        <v>67154</v>
+        <v>62955</v>
       </c>
       <c r="X18" s="13">
-        <f>iferror(lookup(if(W18="",G18,W18),{0,1,10,100,500,1000,5000,10000,25000},{0.0,0.632,0.25,0.149,0.105,0.076,0.043,0.039,0.038}),"")</f>
+        <f>iferror(lookup(if(W18="",G18,W18),{0,1,10,100,500,1000,5000,10000,25000},{0.0,0.632,0.25,0.15,0.105,0.077,0.042,0.039,0.037}),"")</f>
         <v>0</v>
       </c>
       <c r="Y18" s="13">
@@ -2999,13 +2945,13 @@
         <v>0</v>
       </c>
       <c r="AF18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AG18" s="14" t="s">
         <v>106</v>
       </c>
       <c r="AH18">
-        <v>20</v>
+        <v>740</v>
       </c>
       <c r="AJ18" s="13">
         <f>iferror(lookup(if(AI18="",G18,AI18),{0,1,5,50},{0.0,0.238112,0.238112,0.136064}),"")</f>
@@ -3016,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="AL18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AM18" s="14" t="s">
         <v>106</v>
@@ -3054,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1076391</v>
+        <v>26542</v>
       </c>
       <c r="L19" s="13">
         <f>iferror(lookup(if(K19="",G19,K19),{0,1,10,100,500,1000,2500,5000,10000,20000,30000},{0.0,0.1,0.014,0.0062,0.00442,0.00348,0.00316,0.00291,0.00231,0.0022,0.00209}),"")</f>
@@ -3085,10 +3031,10 @@
         <v>106</v>
       </c>
       <c r="V19">
-        <v>270939</v>
+        <v>368890</v>
       </c>
       <c r="X19" s="13">
-        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,100,500,2500,10000},{0.0,0.101,0.006,0.004,0.003,0.002,0.002}),"")</f>
+        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,100,2500,10000},{0.0,0.1,0.006,0.004,0.002,0.002}),"")</f>
         <v>0</v>
       </c>
       <c r="Y19" s="13">
@@ -3110,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG19" s="14" t="s">
         <v>106</v>
@@ -3124,7 +3070,7 @@
         <v>0</v>
       </c>
       <c r="AL19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AM19" s="14" t="s">
         <v>106</v>
@@ -3162,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>30580</v>
+        <v>25477</v>
       </c>
       <c r="L20" s="13">
         <f>iferror(lookup(if(K20="",G20,K20),{0,1,10,100,500,1000,2500,5000,15000,30000},{0.0,0.46,0.316,0.1898,0.14232,0.12018,0.11385,0.10753,0.08525,0.0825}),"")</f>
@@ -3179,10 +3125,10 @@
         <v>106</v>
       </c>
       <c r="V20">
-        <v>26463</v>
+        <v>25053</v>
       </c>
       <c r="X20" s="13">
-        <f>iferror(lookup(if(W20="",G20,W20),{0,1,10,100,500,1000,2500,10000,15000,45000},{0.0,0.401,0.23,0.14,0.127,0.106,0.095,0.086,0.077,0.075}),"")</f>
+        <f>iferror(lookup(if(W20="",G20,W20),{0,1,10,100,500,1000,2500,10000,15000,45000},{0.0,0.401,0.23,0.14,0.126,0.106,0.096,0.086,0.077,0.076}),"")</f>
         <v>0</v>
       </c>
       <c r="Y20" s="13">
@@ -3204,9 +3150,15 @@
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AG20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>180</v>
+      </c>
+      <c r="AM20" s="14" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3273,7 +3225,7 @@
         <v>48671</v>
       </c>
       <c r="X21" s="13">
-        <f>iferror(lookup(if(W21="",G21,W21),{0,1,10,100,10000,30000},{0.0,0.101,0.047,0.026,0.004,0.003}),"")</f>
+        <f>iferror(lookup(if(W21="",G21,W21),{0,1,10,100,10000},{0.0,0.1,0.047,0.026,0.004}),"")</f>
         <v>0</v>
       </c>
       <c r="Y21" s="13">
@@ -3295,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AG21" s="14" t="s">
         <v>106</v>
@@ -3333,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>6616</v>
+        <v>6499</v>
       </c>
       <c r="L22" s="13">
         <f>iferror(lookup(if(K22="",G22,K22),{0,1,10,25,50,100,250,500,1000,5000},{0.0,1.15,1.071,1.02,0.969,0.9435,0.918,0.867,0.816,0.6885}),"")</f>
@@ -3364,10 +3316,10 @@
         <v>106</v>
       </c>
       <c r="V22">
-        <v>2191</v>
+        <v>4336</v>
       </c>
       <c r="X22" s="13">
-        <f>iferror(lookup(if(W22="",G22,W22),{0,1,25,50,100,250,500,1000,2000,5000},{0.0,1.08,1.02,0.969,0.944,0.918,0.867,0.816,0.777,0.689}),"")</f>
+        <f>iferror(lookup(if(W22="",G22,W22),{0,1,25,50,100,250,500,1000,2000,5000},{0.0,1.08,1.02,0.97,0.945,0.919,0.867,0.817,0.778,0.689}),"")</f>
         <v>0</v>
       </c>
       <c r="Y22" s="13">
@@ -3389,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="AF22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG22" s="14" t="s">
         <v>106</v>
@@ -3406,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="AL22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AM22" s="14" t="s">
         <v>106</v>
@@ -3444,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>5914</v>
+        <v>24934</v>
       </c>
       <c r="L23" s="13">
         <f>iferror(lookup(if(K23="",G23,K23),{0,1,10,25,50,100,250,500,1000,5000},{0.0,0.41,0.396,0.3876,0.3466,0.33,0.32176,0.27226,0.264,0.231}),"")</f>
@@ -3475,7 +3427,7 @@
         <v>106</v>
       </c>
       <c r="V23">
-        <v>11403</v>
+        <v>16619</v>
       </c>
       <c r="X23" s="13">
         <f>iferror(lookup(if(W23="",G23,W23),{0,1,10,50,100,200,500,1000,2000},{0.0,0.401,0.393,0.343,0.328,0.319,0.27,0.262,0.23}),"")</f>
@@ -3492,7 +3444,7 @@
         <v>106</v>
       </c>
       <c r="AD23" s="13">
-        <f>iferror(lookup(if(AC23="",G23,AC23),{0,1,250,500,1000,5000},{0.0,0.513,0.387,0.345,0.311,0.282}),"")</f>
+        <f>iferror(lookup(if(AC23="",G23,AC23),{0,1,250,500,1000,5000},{0.0,0.521,0.393,0.351,0.316,0.287}),"")</f>
         <v>0</v>
       </c>
       <c r="AE23" s="13">
@@ -3500,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AG23" s="14" t="s">
         <v>106</v>
@@ -4654,68 +4606,58 @@
     <mergeCell ref="AB5:AG5"/>
     <mergeCell ref="AH5:AM5"/>
   </mergeCells>
-  <conditionalFormatting sqref="AD10">
+  <conditionalFormatting sqref="AD13">
     <cfRule type="cellIs" dxfId="0" priority="97" operator="lessThanOrEqual">
-      <formula>H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD11">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD14">
     <cfRule type="cellIs" dxfId="0" priority="99" operator="lessThanOrEqual">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD13">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD15">
     <cfRule type="cellIs" dxfId="0" priority="101" operator="lessThanOrEqual">
-      <formula>H13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD14">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD16">
     <cfRule type="cellIs" dxfId="0" priority="103" operator="lessThanOrEqual">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD15">
+      <formula>H16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD17">
     <cfRule type="cellIs" dxfId="0" priority="105" operator="lessThanOrEqual">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD16">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD18">
     <cfRule type="cellIs" dxfId="0" priority="107" operator="lessThanOrEqual">
-      <formula>H16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD17">
+      <formula>H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD19">
     <cfRule type="cellIs" dxfId="0" priority="109" operator="lessThanOrEqual">
-      <formula>H17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD18">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD20">
     <cfRule type="cellIs" dxfId="0" priority="111" operator="lessThanOrEqual">
-      <formula>H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD19">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD21">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD20">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD22">
     <cfRule type="cellIs" dxfId="0" priority="115" operator="lessThanOrEqual">
-      <formula>H20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD21">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD23">
     <cfRule type="cellIs" dxfId="0" priority="117" operator="lessThanOrEqual">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD22">
-    <cfRule type="cellIs" dxfId="0" priority="119" operator="lessThanOrEqual">
-      <formula>H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD23">
-    <cfRule type="cellIs" dxfId="0" priority="121" operator="lessThanOrEqual">
       <formula>H23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4729,68 +4671,58 @@
       <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE10">
+  <conditionalFormatting sqref="AE13">
     <cfRule type="cellIs" dxfId="0" priority="98" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE11">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE14">
     <cfRule type="cellIs" dxfId="0" priority="100" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE13">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE15">
     <cfRule type="cellIs" dxfId="0" priority="102" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE14">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE16">
     <cfRule type="cellIs" dxfId="0" priority="104" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE15">
+      <formula>I16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE17">
     <cfRule type="cellIs" dxfId="0" priority="106" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE16">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE18">
     <cfRule type="cellIs" dxfId="0" priority="108" operator="lessThanOrEqual">
-      <formula>I16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE17">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE19">
     <cfRule type="cellIs" dxfId="0" priority="110" operator="lessThanOrEqual">
-      <formula>I17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE18">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE20">
     <cfRule type="cellIs" dxfId="0" priority="112" operator="lessThanOrEqual">
-      <formula>I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE19">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE21">
     <cfRule type="cellIs" dxfId="0" priority="114" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE20">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE22">
     <cfRule type="cellIs" dxfId="0" priority="116" operator="lessThanOrEqual">
-      <formula>I20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE21">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE23">
     <cfRule type="cellIs" dxfId="0" priority="118" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE22">
-    <cfRule type="cellIs" dxfId="0" priority="120" operator="lessThanOrEqual">
-      <formula>I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE23">
-    <cfRule type="cellIs" dxfId="0" priority="122" operator="lessThanOrEqual">
       <formula>I23</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4804,103 +4736,93 @@
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ11">
+  <conditionalFormatting sqref="AJ10">
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="lessThanOrEqual">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ14">
+    <cfRule type="cellIs" dxfId="0" priority="123" operator="lessThanOrEqual">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ15">
     <cfRule type="cellIs" dxfId="0" priority="125" operator="lessThanOrEqual">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ12">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ16">
     <cfRule type="cellIs" dxfId="0" priority="127" operator="lessThanOrEqual">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ14">
+      <formula>H16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ17">
     <cfRule type="cellIs" dxfId="0" priority="129" operator="lessThanOrEqual">
-      <formula>H14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ15">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ18">
     <cfRule type="cellIs" dxfId="0" priority="131" operator="lessThanOrEqual">
-      <formula>H15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ16">
+      <formula>H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ19">
     <cfRule type="cellIs" dxfId="0" priority="133" operator="lessThanOrEqual">
-      <formula>H16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ17">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ22">
     <cfRule type="cellIs" dxfId="0" priority="135" operator="lessThanOrEqual">
-      <formula>H17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ18">
-    <cfRule type="cellIs" dxfId="0" priority="137" operator="lessThanOrEqual">
-      <formula>H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ19">
-    <cfRule type="cellIs" dxfId="0" priority="139" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ22">
-    <cfRule type="cellIs" dxfId="0" priority="141" operator="lessThanOrEqual">
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8">
-    <cfRule type="cellIs" dxfId="0" priority="123" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="119" operator="lessThanOrEqual">
       <formula>H8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK11">
+  <conditionalFormatting sqref="AK10">
+    <cfRule type="cellIs" dxfId="0" priority="122" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK14">
+    <cfRule type="cellIs" dxfId="0" priority="124" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK15">
     <cfRule type="cellIs" dxfId="0" priority="126" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK12">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK16">
     <cfRule type="cellIs" dxfId="0" priority="128" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK14">
+      <formula>I16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK17">
     <cfRule type="cellIs" dxfId="0" priority="130" operator="lessThanOrEqual">
-      <formula>I14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK15">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK18">
     <cfRule type="cellIs" dxfId="0" priority="132" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK16">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK19">
     <cfRule type="cellIs" dxfId="0" priority="134" operator="lessThanOrEqual">
-      <formula>I16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK17">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK22">
     <cfRule type="cellIs" dxfId="0" priority="136" operator="lessThanOrEqual">
-      <formula>I17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK18">
-    <cfRule type="cellIs" dxfId="0" priority="138" operator="lessThanOrEqual">
-      <formula>I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK19">
-    <cfRule type="cellIs" dxfId="0" priority="140" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK22">
-    <cfRule type="cellIs" dxfId="0" priority="142" operator="lessThanOrEqual">
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8">
-    <cfRule type="cellIs" dxfId="0" priority="124" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="120" operator="lessThanOrEqual">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5380,66 +5302,64 @@
     <hyperlink ref="AG9" r:id="rId13"/>
     <hyperlink ref="O10" r:id="rId14"/>
     <hyperlink ref="AA10" r:id="rId15"/>
-    <hyperlink ref="AG10" r:id="rId16"/>
+    <hyperlink ref="AM10" r:id="rId16"/>
     <hyperlink ref="O11" r:id="rId17"/>
     <hyperlink ref="AA11" r:id="rId18"/>
-    <hyperlink ref="AG11" r:id="rId19"/>
-    <hyperlink ref="AM11" r:id="rId20"/>
-    <hyperlink ref="O12" r:id="rId21"/>
-    <hyperlink ref="AA12" r:id="rId22"/>
-    <hyperlink ref="AM12" r:id="rId23"/>
-    <hyperlink ref="O13" r:id="rId24"/>
-    <hyperlink ref="U13" r:id="rId25"/>
-    <hyperlink ref="AA13" r:id="rId26"/>
-    <hyperlink ref="AG13" r:id="rId27"/>
-    <hyperlink ref="O14" r:id="rId28"/>
-    <hyperlink ref="U14" r:id="rId29"/>
-    <hyperlink ref="AA14" r:id="rId30"/>
-    <hyperlink ref="AG14" r:id="rId31"/>
-    <hyperlink ref="AM14" r:id="rId32"/>
-    <hyperlink ref="O15" r:id="rId33"/>
-    <hyperlink ref="U15" r:id="rId34"/>
-    <hyperlink ref="AA15" r:id="rId35"/>
-    <hyperlink ref="AG15" r:id="rId36"/>
-    <hyperlink ref="AM15" r:id="rId37"/>
-    <hyperlink ref="O16" r:id="rId38"/>
-    <hyperlink ref="U16" r:id="rId39"/>
-    <hyperlink ref="AA16" r:id="rId40"/>
-    <hyperlink ref="AG16" r:id="rId41"/>
-    <hyperlink ref="AM16" r:id="rId42"/>
-    <hyperlink ref="O17" r:id="rId43"/>
-    <hyperlink ref="U17" r:id="rId44"/>
-    <hyperlink ref="AA17" r:id="rId45"/>
-    <hyperlink ref="AG17" r:id="rId46"/>
-    <hyperlink ref="AM17" r:id="rId47"/>
-    <hyperlink ref="O18" r:id="rId48"/>
-    <hyperlink ref="U18" r:id="rId49"/>
-    <hyperlink ref="AA18" r:id="rId50"/>
-    <hyperlink ref="AG18" r:id="rId51"/>
-    <hyperlink ref="AM18" r:id="rId52"/>
-    <hyperlink ref="O19" r:id="rId53"/>
-    <hyperlink ref="U19" r:id="rId54"/>
-    <hyperlink ref="AA19" r:id="rId55"/>
-    <hyperlink ref="AG19" r:id="rId56"/>
-    <hyperlink ref="AM19" r:id="rId57"/>
-    <hyperlink ref="O20" r:id="rId58"/>
-    <hyperlink ref="AA20" r:id="rId59"/>
-    <hyperlink ref="AG20" r:id="rId60"/>
-    <hyperlink ref="O21" r:id="rId61"/>
-    <hyperlink ref="U21" r:id="rId62"/>
-    <hyperlink ref="AA21" r:id="rId63"/>
-    <hyperlink ref="AG21" r:id="rId64"/>
-    <hyperlink ref="O22" r:id="rId65"/>
-    <hyperlink ref="U22" r:id="rId66"/>
-    <hyperlink ref="AA22" r:id="rId67"/>
-    <hyperlink ref="AG22" r:id="rId68"/>
-    <hyperlink ref="AM22" r:id="rId69"/>
-    <hyperlink ref="O23" r:id="rId70"/>
-    <hyperlink ref="U23" r:id="rId71"/>
-    <hyperlink ref="AA23" r:id="rId72"/>
-    <hyperlink ref="AG23" r:id="rId73"/>
+    <hyperlink ref="O12" r:id="rId19"/>
+    <hyperlink ref="AA12" r:id="rId20"/>
+    <hyperlink ref="O13" r:id="rId21"/>
+    <hyperlink ref="U13" r:id="rId22"/>
+    <hyperlink ref="AA13" r:id="rId23"/>
+    <hyperlink ref="AG13" r:id="rId24"/>
+    <hyperlink ref="O14" r:id="rId25"/>
+    <hyperlink ref="U14" r:id="rId26"/>
+    <hyperlink ref="AA14" r:id="rId27"/>
+    <hyperlink ref="AG14" r:id="rId28"/>
+    <hyperlink ref="AM14" r:id="rId29"/>
+    <hyperlink ref="O15" r:id="rId30"/>
+    <hyperlink ref="U15" r:id="rId31"/>
+    <hyperlink ref="AA15" r:id="rId32"/>
+    <hyperlink ref="AG15" r:id="rId33"/>
+    <hyperlink ref="AM15" r:id="rId34"/>
+    <hyperlink ref="O16" r:id="rId35"/>
+    <hyperlink ref="U16" r:id="rId36"/>
+    <hyperlink ref="AA16" r:id="rId37"/>
+    <hyperlink ref="AG16" r:id="rId38"/>
+    <hyperlink ref="AM16" r:id="rId39"/>
+    <hyperlink ref="O17" r:id="rId40"/>
+    <hyperlink ref="U17" r:id="rId41"/>
+    <hyperlink ref="AA17" r:id="rId42"/>
+    <hyperlink ref="AG17" r:id="rId43"/>
+    <hyperlink ref="AM17" r:id="rId44"/>
+    <hyperlink ref="O18" r:id="rId45"/>
+    <hyperlink ref="U18" r:id="rId46"/>
+    <hyperlink ref="AA18" r:id="rId47"/>
+    <hyperlink ref="AG18" r:id="rId48"/>
+    <hyperlink ref="AM18" r:id="rId49"/>
+    <hyperlink ref="O19" r:id="rId50"/>
+    <hyperlink ref="U19" r:id="rId51"/>
+    <hyperlink ref="AA19" r:id="rId52"/>
+    <hyperlink ref="AG19" r:id="rId53"/>
+    <hyperlink ref="AM19" r:id="rId54"/>
+    <hyperlink ref="O20" r:id="rId55"/>
+    <hyperlink ref="AA20" r:id="rId56"/>
+    <hyperlink ref="AG20" r:id="rId57"/>
+    <hyperlink ref="AM20" r:id="rId58"/>
+    <hyperlink ref="O21" r:id="rId59"/>
+    <hyperlink ref="U21" r:id="rId60"/>
+    <hyperlink ref="AA21" r:id="rId61"/>
+    <hyperlink ref="AG21" r:id="rId62"/>
+    <hyperlink ref="O22" r:id="rId63"/>
+    <hyperlink ref="U22" r:id="rId64"/>
+    <hyperlink ref="AA22" r:id="rId65"/>
+    <hyperlink ref="AG22" r:id="rId66"/>
+    <hyperlink ref="AM22" r:id="rId67"/>
+    <hyperlink ref="O23" r:id="rId68"/>
+    <hyperlink ref="U23" r:id="rId69"/>
+    <hyperlink ref="AA23" r:id="rId70"/>
+    <hyperlink ref="AG23" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId74"/>
+  <legacyDrawing r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>